<commit_message>
Alten Workflow GT aufgelöst
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
+++ b/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6E9551-32DA-4C62-820C-2BA9ABC34555}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B498FB0-EF8D-409F-AEF3-31F42094BC9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4425" tabRatio="837" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3572,8 +3572,25 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Erstbearbeitung</a:t>
+                <a:t>Erstbearbeitung - erfolgt</a:t>
               </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> immer durch Vertrieb</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="900" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
             </a:p>
             <a:p>
               <a:pPr algn="l"/>
@@ -3651,7 +3668,20 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Organisation eines Präsentationstermins für die Folgewoche und Erfassung des Termins im Teamkalender</a:t>
+                <a:t>Organisation eines Präsentationstermins für die Folgewoche</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Erfassung des Termins im DataFactory Teamkalender ohne Zuordnung zu einer Person</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -3691,6 +3721,19 @@
                   </a:solidFill>
                 </a:rPr>
                 <a:t>Übersendung der Basisprospekte zu den SX Produkten an den Kunden</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Material welches der Kunde sendet wird am Vertriebsticket angehängt, nur bei &gt; 5 MB auf S:\</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -3996,10 +4039,10 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>592049</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>183458</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30074</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>21533</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4018,7 +4061,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3821024" y="7048500"/>
-          <a:ext cx="0" cy="393008"/>
+          <a:ext cx="3248025" cy="421583"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4411,7 +4454,7 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t> Erstpräsentation</a:t>
+                <a:t> Erstpräsentation zu DataFactory Mitarbeter</a:t>
               </a:r>
               <a:endParaRPr lang="de-DE" sz="900" b="1">
                 <a:solidFill>
@@ -4883,6 +4926,28 @@
             </a:p>
             <a:p>
               <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>-&gt; Checkliste Erstpräsentation erstellen, damit alle wichtigen Fragen angesprochen werden</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>-&gt; Dokumentation der Erkenntnisse erfolgt im Vertriebsticket</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
               <a:endParaRPr lang="de-DE" sz="1100" b="0">
                 <a:solidFill>
                   <a:schemeClr val="bg1">
@@ -5257,7 +5322,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="10391775"/>
+          <a:off x="581024" y="10934700"/>
           <a:ext cx="7124700" cy="800101"/>
           <a:chOff x="2895600" y="11839575"/>
           <a:chExt cx="7124700" cy="800101"/>
@@ -5455,7 +5520,7 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Vertriebsticket erstellen</a:t>
+                <a:t>Vertriebsticket aktualisieren</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -5676,7 +5741,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="12496800"/>
+          <a:off x="581024" y="13039725"/>
           <a:ext cx="7191375" cy="1095375"/>
           <a:chOff x="2914650" y="12954000"/>
           <a:chExt cx="7191375" cy="1095375"/>
@@ -6059,16 +6124,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>352421</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>704849</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171445</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -6083,10 +6148,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="8705850"/>
-          <a:ext cx="7162800" cy="1133475"/>
+          <a:off x="3829049" y="8943971"/>
+          <a:ext cx="7162800" cy="1314449"/>
           <a:chOff x="2962275" y="10287000"/>
-          <a:chExt cx="7162800" cy="1133475"/>
+          <a:chExt cx="7162800" cy="888747"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -6219,9 +6284,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="2962275" y="10287000"/>
-            <a:ext cx="6480000" cy="1133475"/>
+            <a:ext cx="6480000" cy="888747"/>
             <a:chOff x="615811" y="11645349"/>
-            <a:chExt cx="7981951" cy="1133475"/>
+            <a:chExt cx="7981951" cy="888747"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -6238,7 +6303,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="615811" y="11905007"/>
-              <a:ext cx="7981951" cy="873817"/>
+              <a:ext cx="7981951" cy="629089"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -6281,7 +6346,7 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Angebot entwickeln &amp; Vertriebsticket erstellen</a:t>
+                <a:t>IndividualAngebot entwickeln </a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -6304,7 +6369,28 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t> Projektkonzepts (Dokument??) </a:t>
+                <a:t> Projektkonzepts (</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>im Dokument??)  </a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Ablage des Konzepts auf S:\</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -6330,7 +6416,7 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Berücksichtigung von Projektmgmt, Testen und Herausarbeiten von Dingen, die nicht Projektbestandteil sind</a:t>
+                <a:t>Berücksichtigung von Projektmgmt</a:t>
               </a:r>
             </a:p>
             <a:p>
@@ -6343,18 +6429,8 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Vertriebsticket in Jira erstellen und Status auf 'Angebot erstellen' setzen</a:t>
+                <a:t>Testen und Herausarbeiten von Dingen, die nicht Projektbestandteil sind</a:t>
               </a:r>
-            </a:p>
-            <a:p>
-              <a:pPr algn="l"/>
-              <a:endParaRPr lang="de-DE" sz="1100" b="0">
-                <a:solidFill>
-                  <a:schemeClr val="bg1">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:endParaRPr>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -6490,7 +6566,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8077200" y="12496800"/>
+          <a:off x="8077200" y="13039725"/>
           <a:ext cx="7124700" cy="800101"/>
           <a:chOff x="11258550" y="11839575"/>
           <a:chExt cx="7124700" cy="800101"/>
@@ -6826,12 +6902,12 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>592049</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>592049</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30074</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>154884</xdr:rowOff>
     </xdr:to>
@@ -6850,9 +6926,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3821024" y="10410825"/>
-          <a:ext cx="0" cy="812109"/>
+        <a:xfrm flipH="1">
+          <a:off x="3821024" y="10258425"/>
+          <a:ext cx="3248025" cy="935934"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -6970,7 +7046,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="14201775"/>
+          <a:off x="581024" y="14744700"/>
           <a:ext cx="7219950" cy="990601"/>
           <a:chOff x="2924175" y="15020925"/>
           <a:chExt cx="7219950" cy="990601"/>
@@ -7371,7 +7447,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="15468600"/>
+          <a:off x="581024" y="16011525"/>
           <a:ext cx="7181850" cy="1190625"/>
           <a:chOff x="2895600" y="16106775"/>
           <a:chExt cx="7181850" cy="1190625"/>
@@ -7545,7 +7621,7 @@
                     </a:schemeClr>
                   </a:solidFill>
                 </a:rPr>
-                <a:t>Projektunterlagen ablegen</a:t>
+                <a:t>Projektunterlagen vom Ticket / Netzlaufwerk ins Repo verschieben</a:t>
               </a:r>
               <a:endParaRPr lang="de-DE" sz="900" b="0">
                 <a:solidFill>
@@ -7781,16 +7857,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>400049</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -7805,10 +7881,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="7181850"/>
-          <a:ext cx="7038975" cy="1428750"/>
+          <a:off x="3829049" y="7210425"/>
+          <a:ext cx="7038975" cy="1504950"/>
           <a:chOff x="2876550" y="8467725"/>
-          <a:chExt cx="7038975" cy="1428750"/>
+          <a:chExt cx="7038975" cy="1504950"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:grpSp>
@@ -7941,9 +8017,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="2876550" y="8467725"/>
-            <a:ext cx="6480000" cy="1428750"/>
+            <a:ext cx="6480000" cy="1504950"/>
             <a:chOff x="615811" y="11645349"/>
-            <a:chExt cx="7981951" cy="1428750"/>
+            <a:chExt cx="7981951" cy="1504950"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -7960,7 +8036,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="615811" y="11905007"/>
-              <a:ext cx="7981951" cy="1169092"/>
+              <a:ext cx="7981951" cy="1245292"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -8083,6 +8159,52 @@
                 </a:rPr>
                 <a:t>Arbeitsmethodik klären (Projektteams, Remotezugang, Rollendefinition)</a:t>
               </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="0" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:uLnTx/>
+                  <a:uFillTx/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>-&gt; Projektmappe anlegen, Dokumentation der Erkenntnisse erfolgt in Projektmappe</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr lang="de-DE" sz="900" b="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
             </a:p>
             <a:p>
               <a:pPr algn="l"/>
@@ -8344,7 +8466,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="18021300"/>
+          <a:off x="581024" y="18564225"/>
           <a:ext cx="7077075" cy="1600200"/>
           <a:chOff x="2914650" y="18545175"/>
           <a:chExt cx="7077075" cy="1600200"/>
@@ -8824,7 +8946,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="16954500"/>
+          <a:off x="581024" y="17497425"/>
           <a:ext cx="7153275" cy="838200"/>
           <a:chOff x="2838450" y="17316450"/>
           <a:chExt cx="7153275" cy="838200"/>
@@ -9209,7 +9331,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="20078700"/>
+          <a:off x="581024" y="20621625"/>
           <a:ext cx="7172325" cy="1228724"/>
           <a:chOff x="3057525" y="20193000"/>
           <a:chExt cx="7172325" cy="1228724"/>
@@ -9643,7 +9765,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="581024" y="21612225"/>
+          <a:off x="581024" y="22155150"/>
           <a:ext cx="7038975" cy="1228724"/>
           <a:chOff x="3028950" y="21574125"/>
           <a:chExt cx="7038975" cy="1228724"/>
@@ -10063,16 +10185,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>592049</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30074</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>592049</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>30074</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>183458</xdr:rowOff>
+      <xdr:rowOff>3032</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -10090,8 +10212,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3821024" y="8610600"/>
-          <a:ext cx="0" cy="354908"/>
+          <a:off x="7069049" y="8715375"/>
+          <a:ext cx="0" cy="612632"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -10772,7 +10894,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>Interessent kontaktiert saxess direkt</a:t>
+            <a:t>- Interessent kontaktiert saxess direkt</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -10785,7 +10907,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>Lead von CP oder anderem Partner</a:t>
+            <a:t>- Lead von CP oder anderem Partner</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -10798,7 +10920,7 @@
                 </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>Lead von CP Partner</a:t>
+            <a:t>- Lead von CP Partner</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -10813,6 +10935,522 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="151" name="Gruppieren 150">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FA2BD37-D214-4993-8763-00707D0312AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="419099" y="7296150"/>
+          <a:ext cx="3019426" cy="990600"/>
+          <a:chOff x="2876550" y="8467725"/>
+          <a:chExt cx="3019426" cy="990600"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="153" name="Gruppieren 152">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA370AE2-FFC9-42B9-ACD3-9B7B3701F23B}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="4876800" y="8810625"/>
+            <a:ext cx="990601" cy="247650"/>
+            <a:chOff x="9353550" y="5648325"/>
+            <a:chExt cx="990601" cy="247650"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="181" name="Grafik 180">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8895E7A0-4D3E-4D1D-8BEE-E61A6FFF5EF4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId7">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="0" b="100000" l="0" r="100000"/>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9353550" y="5657850"/>
+              <a:ext cx="238125" cy="238125"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="183" name="Textfeld 182">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E960CBD-B244-4165-8009-9DF7FD7A50AC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9810750" y="5648325"/>
+              <a:ext cx="533401" cy="161925"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Vertrieb</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="159" name="Gruppieren 158">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A84F0E7-D2A6-408D-A990-F2D75CBF3ADA}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="2876550" y="8467725"/>
+            <a:ext cx="3019426" cy="990600"/>
+            <a:chOff x="615811" y="11645349"/>
+            <a:chExt cx="3719277" cy="990600"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="170" name="Rechteck 169">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79951AF9-97C1-48E3-96ED-C68D15523CE2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="615811" y="11905007"/>
+              <a:ext cx="3719277" cy="730942"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Direktangebot Standard</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="1" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t> Solution</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="900" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>- Angebot </a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>- Systemvoraussetzungen</a:t>
+              </a:r>
+            </a:p>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900" b="0">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>- AGB</a:t>
+              </a:r>
+              <a:endParaRPr lang="de-DE" sz="1100" b="0">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="171" name="Grafik 170">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AAA4E2FC-1795-4A22-85DF-DF6B42F9B7B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noChangeAspect="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+              <a:extLst>
+                <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+                  <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                    <a14:imgLayer r:embed="rId5">
+                      <a14:imgEffect>
+                        <a14:backgroundRemoval t="0" b="100000" l="0" r="100000">
+                          <a14:foregroundMark x1="42222" y1="45333" x2="59556" y2="52889"/>
+                          <a14:foregroundMark x1="72444" y1="43556" x2="92889" y2="52444"/>
+                          <a14:foregroundMark x1="79556" y1="40000" x2="92444" y2="40444"/>
+                          <a14:foregroundMark x1="95111" y1="41778" x2="97778" y2="47556"/>
+                          <a14:foregroundMark x1="78222" y1="59111" x2="87111" y2="59111"/>
+                        </a14:backgroundRemoval>
+                      </a14:imgEffect>
+                    </a14:imgLayer>
+                  </a14:imgProps>
+                </a:ext>
+              </a:extLst>
+            </a:blip>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="646044" y="11645349"/>
+              <a:ext cx="314739" cy="314739"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="180" name="Textfeld 179">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628F558E-9567-4065-82B2-B15FCD323565}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1018761" y="11728174"/>
+              <a:ext cx="866775" cy="174550"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="de-DE" sz="900">
+                  <a:solidFill>
+                    <a:schemeClr val="bg1">
+                      <a:lumMod val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>Prozessschritt</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>592049</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>107258</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="184" name="Gerade Verbindung mit Pfeil 183">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B2A9B3-082E-4095-9416-F736B72A8B4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="2"/>
+          <a:endCxn id="170" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1928812" y="7048500"/>
+          <a:ext cx="1892212" cy="507308"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>592049</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>154884</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="185" name="Gerade Verbindung mit Pfeil 184">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13972B34-D612-4E75-9A57-E2577B35C626}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="170" idx="2"/>
+          <a:endCxn id="148" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1928812" y="8286750"/>
+          <a:ext cx="1892212" cy="2907609"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -28922,7 +29560,7 @@
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L19" sqref="L19"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29045,12 +29683,12 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L19" sqref="L19"/>
-      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
+      <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29161,6 +29799,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
+    <row r="45" ht="57.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Punkte aus Besprechung Mandy / Helga ergänzt
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
+++ b/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF567AC-71C0-45AC-82AD-D23468A8C72A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B071EC-79FD-4D54-8CC7-6405E11EB45A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4425" tabRatio="837" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,22 +15,17 @@
     <sheet name="Projektverlauf" sheetId="53" r:id="rId5"/>
     <sheet name="Corporate Design" sheetId="52" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Abgeschlossen</t>
   </si>
@@ -162,6 +157,12 @@
   </si>
   <si>
     <t>Jira Abbildung Workflow</t>
+  </si>
+  <si>
+    <t>Offene Fragen ?</t>
+  </si>
+  <si>
+    <t>Installation läßt sich nicht einfach DF und SXI zuordnen - wie umgehen ?</t>
   </si>
 </sst>
 </file>
@@ -937,8 +938,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>23813</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -953,8 +954,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4881562" y="4126855"/>
-          <a:ext cx="3262313" cy="1935808"/>
+          <a:off x="4605337" y="4288780"/>
+          <a:ext cx="3052763" cy="2750195"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1114,16 +1115,25 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="900" b="0" baseline="0">
+            <a:rPr lang="de-DE" sz="900" b="1">
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
             </a:rPr>
-            <a:t>- Zeiten vom Typ Installation ?</a:t>
+            <a:t>Projektaufgabe</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> = Projektplan = Projektleiter = Projektabrechnung über SXI und DF</a:t>
+          </a:r>
           <a:endParaRPr lang="de-DE" sz="900" b="1">
             <a:solidFill>
               <a:schemeClr val="bg1">
@@ -1146,8 +1156,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>280987</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1162,8 +1172,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8258175" y="4126855"/>
-          <a:ext cx="3619500" cy="1950095"/>
+          <a:off x="7772400" y="4288780"/>
+          <a:ext cx="3357562" cy="2721620"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1508,15 +1518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>633413</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>73968</xdr:rowOff>
+      <xdr:colOff>623888</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>188268</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1531,8 +1541,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4900613" y="6293793"/>
-          <a:ext cx="7019925" cy="545157"/>
+          <a:off x="4614863" y="7255818"/>
+          <a:ext cx="6548437" cy="573732"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -28016,17 +28026,17 @@
       <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.3984375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -28049,7 +28059,7 @@
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -28074,7 +28084,7 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>28</v>
@@ -28101,7 +28111,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -28124,12 +28134,12 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
@@ -28137,10 +28147,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
@@ -28148,10 +28158,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>39</v>
       </c>
@@ -28159,17 +28169,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="8"/>
       <c r="E17" s="25"/>
     </row>
@@ -28199,22 +28209,22 @@
       <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.73046875" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
-    <col min="9" max="11" width="15.73046875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="29.265625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="9"/>
-    <col min="14" max="14" width="50.73046875" style="9" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="11" width="15.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="29.28515625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="9"/>
+    <col min="14" max="14" width="50.7109375" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -28230,7 +28240,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>26</v>
@@ -28248,7 +28258,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="str">
         <f>Übersicht!B3</f>
@@ -28269,7 +28279,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -28285,7 +28295,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I6" s="15" t="s">
         <v>6</v>
       </c>
@@ -28299,7 +28309,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="35"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I7" s="13" t="s">
         <v>1</v>
       </c>
@@ -28319,7 +28329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -28327,7 +28337,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="35"/>
     </row>
-    <row r="9" spans="1:14" collapsed="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
         <v>0</v>
       </c>
@@ -28344,7 +28354,7 @@
       <c r="M9" s="33"/>
       <c r="N9" s="36"/>
     </row>
-    <row r="10" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -28352,7 +28362,7 @@
       <c r="M10" s="21"/>
       <c r="N10" s="35"/>
     </row>
-    <row r="11" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B11" s="26" t="s">
         <v>23</v>
       </c>
@@ -28371,7 +28381,7 @@
       <c r="M11" s="30"/>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:14" s="4" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B12" s="40"/>
       <c r="H12" s="41"/>
       <c r="I12" s="42"/>
@@ -28381,7 +28391,7 @@
       <c r="M12" s="43"/>
       <c r="N12" s="44"/>
     </row>
-    <row r="13" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B13" s="17">
         <v>1</v>
       </c>
@@ -28406,7 +28416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
@@ -28420,7 +28430,7 @@
       <c r="M14" s="21"/>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C15" s="18" t="s">
         <v>14</v>
       </c>
@@ -28431,7 +28441,7 @@
       <c r="M15" s="21"/>
       <c r="N15" s="35"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -28439,7 +28449,7 @@
       <c r="M16" s="21"/>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -28447,7 +28457,7 @@
       <c r="M17" s="21"/>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="s">
         <v>21</v>
       </c>
@@ -28464,7 +28474,7 @@
       <c r="M18" s="33"/>
       <c r="N18" s="36"/>
     </row>
-    <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -28472,7 +28482,7 @@
       <c r="M19" s="21"/>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>29</v>
       </c>
@@ -28491,7 +28501,7 @@
       <c r="M20" s="30"/>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -28499,7 +28509,7 @@
       <c r="M21" s="21"/>
       <c r="N21" s="35"/>
     </row>
-    <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B22" s="17">
         <v>1</v>
       </c>
@@ -28520,7 +28530,7 @@
       <c r="M22" s="21"/>
       <c r="N22" s="38"/>
     </row>
-    <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
         <v>30</v>
       </c>
@@ -28534,7 +28544,7 @@
       <c r="M23" s="21"/>
       <c r="N23" s="38"/>
     </row>
-    <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C24" s="18" t="s">
         <v>35</v>
       </c>
@@ -28545,7 +28555,7 @@
       <c r="M24" s="21"/>
       <c r="N24" s="35"/>
     </row>
-    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
@@ -28553,7 +28563,7 @@
       <c r="M25" s="21"/>
       <c r="N25" s="35"/>
     </row>
-    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>2</v>
       </c>
@@ -28574,7 +28584,7 @@
       <c r="M26" s="21"/>
       <c r="N26" s="38"/>
     </row>
-    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
         <v>32</v>
       </c>
@@ -28588,7 +28598,7 @@
       <c r="M27" s="21"/>
       <c r="N27" s="38"/>
     </row>
-    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C28" s="18" t="s">
         <v>37</v>
       </c>
@@ -28599,7 +28609,7 @@
       <c r="M28" s="21"/>
       <c r="N28" s="35"/>
     </row>
-    <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C29" s="18"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -28608,7 +28618,7 @@
       <c r="M29" s="21"/>
       <c r="N29" s="35"/>
     </row>
-    <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C30" s="18"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -28617,7 +28627,7 @@
       <c r="M30" s="21"/>
       <c r="N30" s="35"/>
     </row>
-    <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C31" s="18"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -28626,7 +28636,7 @@
       <c r="M31" s="21"/>
       <c r="N31" s="35"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C32" s="18"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -28635,7 +28645,7 @@
       <c r="M32" s="21"/>
       <c r="N32" s="35"/>
     </row>
-    <row r="33" spans="2:14" collapsed="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
       <c r="B33" s="31" t="s">
         <v>18</v>
       </c>
@@ -28652,7 +28662,7 @@
       <c r="M33" s="33"/>
       <c r="N33" s="36"/>
     </row>
-    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
@@ -28660,7 +28670,7 @@
       <c r="M34" s="21"/>
       <c r="N34" s="35"/>
     </row>
-    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B35" s="17" t="s">
         <v>10</v>
       </c>
@@ -28687,7 +28697,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B36" s="16"/>
       <c r="C36" s="18" t="s">
         <v>16</v>
@@ -28699,7 +28709,7 @@
       <c r="M36" s="21"/>
       <c r="N36" s="38"/>
     </row>
-    <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C37" s="18" t="s">
         <v>16</v>
       </c>
@@ -28710,7 +28720,7 @@
       <c r="M37" s="21"/>
       <c r="N37" s="35"/>
     </row>
-    <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C38" s="18" t="s">
         <v>16</v>
       </c>
@@ -28721,7 +28731,7 @@
       <c r="M38" s="21"/>
       <c r="N38" s="35"/>
     </row>
-    <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C39" s="18" t="s">
         <v>16</v>
       </c>
@@ -28732,7 +28742,7 @@
       <c r="M39" s="21"/>
       <c r="N39" s="35"/>
     </row>
-    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
@@ -28740,7 +28750,7 @@
       <c r="M40" s="21"/>
       <c r="N40" s="35"/>
     </row>
-    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
@@ -28748,7 +28758,7 @@
       <c r="M41" s="21"/>
       <c r="N41" s="35"/>
     </row>
-    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
@@ -28756,7 +28766,7 @@
       <c r="M42" s="21"/>
       <c r="N42" s="35"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
@@ -28764,1707 +28774,1707 @@
       <c r="M43" s="22"/>
       <c r="N43" s="39"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
       <c r="K47" s="20"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
       <c r="K48" s="20"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
     </row>
-    <row r="49" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="49" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
       <c r="K49" s="20"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
     </row>
-    <row r="50" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="50" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
       <c r="K50" s="20"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
     </row>
-    <row r="51" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="51" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
     </row>
-    <row r="52" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="52" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
-    <row r="53" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="53" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
     </row>
-    <row r="54" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="54" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
       <c r="K54" s="20"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
     </row>
-    <row r="55" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="55" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I55" s="20"/>
       <c r="J55" s="20"/>
       <c r="K55" s="20"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
     </row>
-    <row r="56" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="56" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
       <c r="K56" s="20"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
     </row>
-    <row r="57" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="57" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
       <c r="L57" s="22"/>
       <c r="M57" s="22"/>
     </row>
-    <row r="58" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="58" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
       <c r="K58" s="20"/>
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
     </row>
-    <row r="59" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="59" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
       <c r="L59" s="22"/>
       <c r="M59" s="22"/>
     </row>
-    <row r="60" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="60" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
       <c r="K60" s="20"/>
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
     </row>
-    <row r="61" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="61" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
       <c r="K61" s="20"/>
       <c r="L61" s="22"/>
       <c r="M61" s="22"/>
     </row>
-    <row r="62" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="62" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I62" s="20"/>
       <c r="J62" s="20"/>
       <c r="K62" s="20"/>
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
     </row>
-    <row r="63" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="63" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I63" s="20"/>
       <c r="J63" s="20"/>
       <c r="K63" s="20"/>
       <c r="L63" s="22"/>
       <c r="M63" s="22"/>
     </row>
-    <row r="64" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="64" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
       <c r="K64" s="20"/>
       <c r="L64" s="22"/>
       <c r="M64" s="22"/>
     </row>
-    <row r="65" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="65" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I65" s="20"/>
       <c r="J65" s="20"/>
       <c r="K65" s="20"/>
       <c r="L65" s="22"/>
       <c r="M65" s="22"/>
     </row>
-    <row r="66" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="66" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
       <c r="K66" s="20"/>
       <c r="L66" s="22"/>
       <c r="M66" s="22"/>
     </row>
-    <row r="67" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="67" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I67" s="20"/>
       <c r="J67" s="20"/>
       <c r="K67" s="20"/>
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
     </row>
-    <row r="68" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="68" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I68" s="20"/>
       <c r="J68" s="20"/>
       <c r="K68" s="20"/>
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
     </row>
-    <row r="69" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="69" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
     </row>
-    <row r="70" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="70" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
     </row>
-    <row r="71" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="71" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
       <c r="K71" s="20"/>
       <c r="L71" s="22"/>
       <c r="M71" s="22"/>
     </row>
-    <row r="72" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="72" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
       <c r="K72" s="20"/>
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
     </row>
-    <row r="73" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="73" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
       <c r="K73" s="20"/>
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
     </row>
-    <row r="74" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="74" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I74" s="20"/>
       <c r="J74" s="20"/>
       <c r="K74" s="20"/>
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
     </row>
-    <row r="75" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="75" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I75" s="20"/>
       <c r="J75" s="20"/>
       <c r="K75" s="20"/>
       <c r="L75" s="22"/>
       <c r="M75" s="22"/>
     </row>
-    <row r="76" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="76" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
       <c r="K76" s="20"/>
       <c r="L76" s="22"/>
       <c r="M76" s="22"/>
     </row>
-    <row r="77" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="77" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I77" s="20"/>
       <c r="J77" s="20"/>
       <c r="K77" s="20"/>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>
     </row>
-    <row r="78" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="78" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I78" s="20"/>
       <c r="J78" s="20"/>
       <c r="K78" s="20"/>
       <c r="L78" s="22"/>
       <c r="M78" s="22"/>
     </row>
-    <row r="79" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="79" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I79" s="20"/>
       <c r="J79" s="20"/>
       <c r="K79" s="20"/>
       <c r="L79" s="22"/>
       <c r="M79" s="22"/>
     </row>
-    <row r="80" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="80" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I80" s="20"/>
       <c r="J80" s="20"/>
       <c r="K80" s="20"/>
       <c r="L80" s="22"/>
       <c r="M80" s="22"/>
     </row>
-    <row r="81" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="81" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
       <c r="K81" s="20"/>
       <c r="L81" s="22"/>
       <c r="M81" s="22"/>
     </row>
-    <row r="82" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="82" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I82" s="20"/>
       <c r="J82" s="20"/>
       <c r="K82" s="20"/>
       <c r="L82" s="22"/>
       <c r="M82" s="22"/>
     </row>
-    <row r="83" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="83" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I83" s="20"/>
       <c r="J83" s="20"/>
       <c r="K83" s="20"/>
       <c r="L83" s="22"/>
       <c r="M83" s="22"/>
     </row>
-    <row r="84" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="84" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I84" s="20"/>
       <c r="J84" s="20"/>
       <c r="K84" s="20"/>
       <c r="L84" s="22"/>
       <c r="M84" s="22"/>
     </row>
-    <row r="85" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="85" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I85" s="20"/>
       <c r="J85" s="20"/>
       <c r="K85" s="20"/>
       <c r="L85" s="22"/>
       <c r="M85" s="22"/>
     </row>
-    <row r="86" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="86" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I86" s="20"/>
       <c r="J86" s="20"/>
       <c r="K86" s="20"/>
       <c r="L86" s="22"/>
       <c r="M86" s="22"/>
     </row>
-    <row r="87" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="87" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I87" s="20"/>
       <c r="J87" s="20"/>
       <c r="K87" s="20"/>
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
     </row>
-    <row r="88" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="88" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I88" s="20"/>
       <c r="J88" s="20"/>
       <c r="K88" s="20"/>
       <c r="L88" s="22"/>
       <c r="M88" s="22"/>
     </row>
-    <row r="89" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="89" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I89" s="20"/>
       <c r="J89" s="20"/>
       <c r="K89" s="20"/>
       <c r="L89" s="22"/>
       <c r="M89" s="22"/>
     </row>
-    <row r="90" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="90" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I90" s="20"/>
       <c r="J90" s="20"/>
       <c r="K90" s="20"/>
       <c r="L90" s="22"/>
       <c r="M90" s="22"/>
     </row>
-    <row r="91" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="91" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I91" s="20"/>
       <c r="J91" s="20"/>
       <c r="K91" s="20"/>
       <c r="L91" s="22"/>
       <c r="M91" s="22"/>
     </row>
-    <row r="92" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="92" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I92" s="20"/>
       <c r="J92" s="20"/>
       <c r="K92" s="20"/>
       <c r="L92" s="22"/>
       <c r="M92" s="22"/>
     </row>
-    <row r="93" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="93" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I93" s="20"/>
       <c r="J93" s="20"/>
       <c r="K93" s="20"/>
       <c r="L93" s="22"/>
       <c r="M93" s="22"/>
     </row>
-    <row r="94" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="94" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I94" s="20"/>
       <c r="J94" s="20"/>
       <c r="K94" s="20"/>
       <c r="L94" s="22"/>
       <c r="M94" s="22"/>
     </row>
-    <row r="95" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="95" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I95" s="20"/>
       <c r="J95" s="20"/>
       <c r="K95" s="20"/>
       <c r="L95" s="22"/>
       <c r="M95" s="22"/>
     </row>
-    <row r="96" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="96" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
       <c r="K96" s="20"/>
       <c r="L96" s="22"/>
       <c r="M96" s="22"/>
     </row>
-    <row r="97" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="97" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I97" s="20"/>
       <c r="J97" s="20"/>
       <c r="K97" s="20"/>
       <c r="L97" s="22"/>
       <c r="M97" s="22"/>
     </row>
-    <row r="98" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="98" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I98" s="20"/>
       <c r="J98" s="20"/>
       <c r="K98" s="20"/>
       <c r="L98" s="22"/>
       <c r="M98" s="22"/>
     </row>
-    <row r="99" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="99" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I99" s="20"/>
       <c r="J99" s="20"/>
       <c r="K99" s="20"/>
       <c r="L99" s="22"/>
       <c r="M99" s="22"/>
     </row>
-    <row r="100" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="100" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I100" s="20"/>
       <c r="J100" s="20"/>
       <c r="K100" s="20"/>
       <c r="L100" s="22"/>
       <c r="M100" s="22"/>
     </row>
-    <row r="101" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="101" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I101" s="20"/>
       <c r="J101" s="20"/>
       <c r="K101" s="20"/>
       <c r="L101" s="22"/>
       <c r="M101" s="22"/>
     </row>
-    <row r="102" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="102" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I102" s="20"/>
       <c r="J102" s="20"/>
       <c r="K102" s="20"/>
       <c r="L102" s="22"/>
       <c r="M102" s="22"/>
     </row>
-    <row r="103" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="103" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I103" s="20"/>
       <c r="J103" s="20"/>
       <c r="K103" s="20"/>
       <c r="L103" s="22"/>
       <c r="M103" s="22"/>
     </row>
-    <row r="104" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="104" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I104" s="20"/>
       <c r="J104" s="20"/>
       <c r="K104" s="20"/>
       <c r="L104" s="22"/>
       <c r="M104" s="22"/>
     </row>
-    <row r="105" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="105" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I105" s="20"/>
       <c r="J105" s="20"/>
       <c r="K105" s="20"/>
       <c r="L105" s="22"/>
       <c r="M105" s="22"/>
     </row>
-    <row r="106" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="106" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I106" s="20"/>
       <c r="J106" s="20"/>
       <c r="K106" s="20"/>
       <c r="L106" s="22"/>
       <c r="M106" s="22"/>
     </row>
-    <row r="107" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="107" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I107" s="20"/>
       <c r="J107" s="20"/>
       <c r="K107" s="20"/>
       <c r="L107" s="22"/>
       <c r="M107" s="22"/>
     </row>
-    <row r="108" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="108" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I108" s="20"/>
       <c r="J108" s="20"/>
       <c r="K108" s="20"/>
       <c r="L108" s="22"/>
       <c r="M108" s="22"/>
     </row>
-    <row r="109" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="109" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I109" s="20"/>
       <c r="J109" s="20"/>
       <c r="K109" s="20"/>
       <c r="L109" s="22"/>
       <c r="M109" s="22"/>
     </row>
-    <row r="110" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="110" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I110" s="20"/>
       <c r="J110" s="20"/>
       <c r="K110" s="20"/>
       <c r="L110" s="22"/>
       <c r="M110" s="22"/>
     </row>
-    <row r="111" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="111" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I111" s="20"/>
       <c r="J111" s="20"/>
       <c r="K111" s="20"/>
       <c r="L111" s="22"/>
       <c r="M111" s="22"/>
     </row>
-    <row r="112" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="112" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I112" s="20"/>
       <c r="J112" s="20"/>
       <c r="K112" s="20"/>
       <c r="L112" s="22"/>
       <c r="M112" s="22"/>
     </row>
-    <row r="113" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="113" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I113" s="20"/>
       <c r="J113" s="20"/>
       <c r="K113" s="20"/>
       <c r="L113" s="22"/>
       <c r="M113" s="22"/>
     </row>
-    <row r="114" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="114" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
       <c r="K114" s="20"/>
       <c r="L114" s="22"/>
       <c r="M114" s="22"/>
     </row>
-    <row r="115" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="115" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I115" s="20"/>
       <c r="J115" s="20"/>
       <c r="K115" s="20"/>
       <c r="L115" s="22"/>
       <c r="M115" s="22"/>
     </row>
-    <row r="116" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="116" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I116" s="20"/>
       <c r="J116" s="20"/>
       <c r="K116" s="20"/>
       <c r="L116" s="22"/>
       <c r="M116" s="22"/>
     </row>
-    <row r="117" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="117" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I117" s="20"/>
       <c r="J117" s="20"/>
       <c r="K117" s="20"/>
       <c r="L117" s="22"/>
       <c r="M117" s="22"/>
     </row>
-    <row r="118" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="118" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
       <c r="K118" s="20"/>
       <c r="L118" s="22"/>
       <c r="M118" s="22"/>
     </row>
-    <row r="119" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="119" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
       <c r="K119" s="20"/>
       <c r="L119" s="22"/>
       <c r="M119" s="22"/>
     </row>
-    <row r="120" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="120" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I120" s="20"/>
       <c r="J120" s="20"/>
       <c r="K120" s="20"/>
       <c r="L120" s="22"/>
       <c r="M120" s="22"/>
     </row>
-    <row r="121" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="121" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I121" s="20"/>
       <c r="J121" s="20"/>
       <c r="K121" s="20"/>
       <c r="L121" s="22"/>
       <c r="M121" s="22"/>
     </row>
-    <row r="122" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="122" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I122" s="20"/>
       <c r="J122" s="20"/>
       <c r="K122" s="20"/>
       <c r="L122" s="22"/>
       <c r="M122" s="22"/>
     </row>
-    <row r="123" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="123" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
       <c r="K123" s="20"/>
       <c r="L123" s="22"/>
       <c r="M123" s="22"/>
     </row>
-    <row r="124" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="124" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I124" s="20"/>
       <c r="J124" s="20"/>
       <c r="K124" s="20"/>
       <c r="L124" s="22"/>
       <c r="M124" s="22"/>
     </row>
-    <row r="125" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="125" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
       <c r="K125" s="20"/>
       <c r="L125" s="22"/>
       <c r="M125" s="22"/>
     </row>
-    <row r="126" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="126" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
       <c r="K126" s="20"/>
       <c r="L126" s="22"/>
       <c r="M126" s="22"/>
     </row>
-    <row r="127" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="127" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
       <c r="K127" s="20"/>
       <c r="L127" s="22"/>
       <c r="M127" s="22"/>
     </row>
-    <row r="128" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="128" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
       <c r="K128" s="20"/>
       <c r="L128" s="22"/>
       <c r="M128" s="22"/>
     </row>
-    <row r="129" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="129" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
       <c r="K129" s="20"/>
       <c r="L129" s="22"/>
       <c r="M129" s="22"/>
     </row>
-    <row r="130" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="130" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
       <c r="L130" s="22"/>
       <c r="M130" s="22"/>
     </row>
-    <row r="131" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="131" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
       <c r="K131" s="20"/>
       <c r="L131" s="22"/>
       <c r="M131" s="22"/>
     </row>
-    <row r="132" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="132" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I132" s="20"/>
       <c r="J132" s="20"/>
       <c r="K132" s="20"/>
       <c r="L132" s="22"/>
       <c r="M132" s="22"/>
     </row>
-    <row r="133" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="133" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I133" s="20"/>
       <c r="J133" s="20"/>
       <c r="K133" s="20"/>
       <c r="L133" s="22"/>
       <c r="M133" s="22"/>
     </row>
-    <row r="134" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="134" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I134" s="20"/>
       <c r="J134" s="20"/>
       <c r="K134" s="20"/>
       <c r="L134" s="22"/>
       <c r="M134" s="22"/>
     </row>
-    <row r="135" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="135" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I135" s="20"/>
       <c r="J135" s="20"/>
       <c r="K135" s="20"/>
       <c r="L135" s="22"/>
       <c r="M135" s="22"/>
     </row>
-    <row r="136" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="136" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I136" s="20"/>
       <c r="J136" s="20"/>
       <c r="K136" s="20"/>
       <c r="L136" s="22"/>
       <c r="M136" s="22"/>
     </row>
-    <row r="137" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="137" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I137" s="20"/>
       <c r="J137" s="20"/>
       <c r="K137" s="20"/>
       <c r="L137" s="22"/>
       <c r="M137" s="22"/>
     </row>
-    <row r="138" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="138" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I138" s="20"/>
       <c r="J138" s="20"/>
       <c r="K138" s="20"/>
       <c r="L138" s="22"/>
       <c r="M138" s="22"/>
     </row>
-    <row r="139" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="139" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I139" s="20"/>
       <c r="J139" s="20"/>
       <c r="K139" s="20"/>
       <c r="L139" s="22"/>
       <c r="M139" s="22"/>
     </row>
-    <row r="140" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="140" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I140" s="20"/>
       <c r="J140" s="20"/>
       <c r="K140" s="20"/>
       <c r="L140" s="22"/>
       <c r="M140" s="22"/>
     </row>
-    <row r="141" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="141" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I141" s="20"/>
       <c r="J141" s="20"/>
       <c r="K141" s="20"/>
       <c r="L141" s="22"/>
       <c r="M141" s="22"/>
     </row>
-    <row r="142" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="142" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I142" s="20"/>
       <c r="J142" s="20"/>
       <c r="K142" s="20"/>
       <c r="L142" s="22"/>
       <c r="M142" s="22"/>
     </row>
-    <row r="143" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="143" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I143" s="20"/>
       <c r="J143" s="20"/>
       <c r="K143" s="20"/>
       <c r="L143" s="22"/>
       <c r="M143" s="22"/>
     </row>
-    <row r="144" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="144" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I144" s="20"/>
       <c r="J144" s="20"/>
       <c r="K144" s="20"/>
       <c r="L144" s="22"/>
       <c r="M144" s="22"/>
     </row>
-    <row r="145" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="145" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I145" s="20"/>
       <c r="J145" s="20"/>
       <c r="K145" s="20"/>
       <c r="L145" s="22"/>
       <c r="M145" s="22"/>
     </row>
-    <row r="146" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="146" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I146" s="20"/>
       <c r="J146" s="20"/>
       <c r="K146" s="20"/>
       <c r="L146" s="22"/>
       <c r="M146" s="22"/>
     </row>
-    <row r="147" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="147" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I147" s="20"/>
       <c r="J147" s="20"/>
       <c r="K147" s="20"/>
       <c r="L147" s="22"/>
       <c r="M147" s="22"/>
     </row>
-    <row r="148" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="148" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I148" s="20"/>
       <c r="J148" s="20"/>
       <c r="K148" s="20"/>
       <c r="L148" s="22"/>
       <c r="M148" s="22"/>
     </row>
-    <row r="149" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="149" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I149" s="20"/>
       <c r="J149" s="20"/>
       <c r="K149" s="20"/>
       <c r="L149" s="22"/>
       <c r="M149" s="22"/>
     </row>
-    <row r="150" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="150" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I150" s="20"/>
       <c r="J150" s="20"/>
       <c r="K150" s="20"/>
       <c r="L150" s="22"/>
       <c r="M150" s="22"/>
     </row>
-    <row r="151" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="151" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I151" s="20"/>
       <c r="J151" s="20"/>
       <c r="K151" s="20"/>
       <c r="L151" s="22"/>
       <c r="M151" s="22"/>
     </row>
-    <row r="152" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="152" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I152" s="20"/>
       <c r="J152" s="20"/>
       <c r="K152" s="20"/>
       <c r="L152" s="22"/>
       <c r="M152" s="22"/>
     </row>
-    <row r="153" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="153" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I153" s="20"/>
       <c r="J153" s="20"/>
       <c r="K153" s="20"/>
       <c r="L153" s="22"/>
       <c r="M153" s="22"/>
     </row>
-    <row r="154" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="154" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I154" s="20"/>
       <c r="J154" s="20"/>
       <c r="K154" s="20"/>
       <c r="L154" s="22"/>
       <c r="M154" s="22"/>
     </row>
-    <row r="155" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="155" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I155" s="20"/>
       <c r="J155" s="20"/>
       <c r="K155" s="20"/>
       <c r="L155" s="22"/>
       <c r="M155" s="22"/>
     </row>
-    <row r="156" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="156" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I156" s="20"/>
       <c r="J156" s="20"/>
       <c r="K156" s="20"/>
       <c r="L156" s="22"/>
       <c r="M156" s="22"/>
     </row>
-    <row r="157" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="157" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I157" s="20"/>
       <c r="J157" s="20"/>
       <c r="K157" s="20"/>
       <c r="L157" s="22"/>
       <c r="M157" s="22"/>
     </row>
-    <row r="158" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="158" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I158" s="20"/>
       <c r="J158" s="20"/>
       <c r="K158" s="20"/>
       <c r="L158" s="22"/>
       <c r="M158" s="22"/>
     </row>
-    <row r="159" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="159" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I159" s="20"/>
       <c r="J159" s="20"/>
       <c r="K159" s="20"/>
       <c r="L159" s="22"/>
       <c r="M159" s="22"/>
     </row>
-    <row r="160" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="160" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I160" s="20"/>
       <c r="J160" s="20"/>
       <c r="K160" s="20"/>
       <c r="L160" s="22"/>
       <c r="M160" s="22"/>
     </row>
-    <row r="161" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="161" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I161" s="20"/>
       <c r="J161" s="20"/>
       <c r="K161" s="20"/>
       <c r="L161" s="22"/>
       <c r="M161" s="22"/>
     </row>
-    <row r="162" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="162" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I162" s="20"/>
       <c r="J162" s="20"/>
       <c r="K162" s="20"/>
       <c r="L162" s="22"/>
       <c r="M162" s="22"/>
     </row>
-    <row r="163" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="163" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I163" s="20"/>
       <c r="J163" s="20"/>
       <c r="K163" s="20"/>
       <c r="L163" s="22"/>
       <c r="M163" s="22"/>
     </row>
-    <row r="164" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="164" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I164" s="20"/>
       <c r="J164" s="20"/>
       <c r="K164" s="20"/>
       <c r="L164" s="22"/>
       <c r="M164" s="22"/>
     </row>
-    <row r="165" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="165" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I165" s="20"/>
       <c r="J165" s="20"/>
       <c r="K165" s="20"/>
       <c r="L165" s="22"/>
       <c r="M165" s="22"/>
     </row>
-    <row r="166" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="166" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I166" s="20"/>
       <c r="J166" s="20"/>
       <c r="K166" s="20"/>
       <c r="L166" s="22"/>
       <c r="M166" s="22"/>
     </row>
-    <row r="167" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="167" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I167" s="20"/>
       <c r="J167" s="20"/>
       <c r="K167" s="20"/>
       <c r="L167" s="22"/>
       <c r="M167" s="22"/>
     </row>
-    <row r="168" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="168" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I168" s="20"/>
       <c r="J168" s="20"/>
       <c r="K168" s="20"/>
       <c r="L168" s="22"/>
       <c r="M168" s="22"/>
     </row>
-    <row r="169" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="169" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I169" s="20"/>
       <c r="J169" s="20"/>
       <c r="K169" s="20"/>
       <c r="L169" s="22"/>
       <c r="M169" s="22"/>
     </row>
-    <row r="170" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="170" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I170" s="20"/>
       <c r="J170" s="20"/>
       <c r="K170" s="20"/>
       <c r="L170" s="22"/>
       <c r="M170" s="22"/>
     </row>
-    <row r="171" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="171" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I171" s="20"/>
       <c r="J171" s="20"/>
       <c r="K171" s="20"/>
       <c r="L171" s="22"/>
       <c r="M171" s="22"/>
     </row>
-    <row r="172" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="172" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I172" s="20"/>
       <c r="J172" s="20"/>
       <c r="K172" s="20"/>
       <c r="L172" s="22"/>
       <c r="M172" s="22"/>
     </row>
-    <row r="173" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="173" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I173" s="20"/>
       <c r="J173" s="20"/>
       <c r="K173" s="20"/>
       <c r="L173" s="22"/>
       <c r="M173" s="22"/>
     </row>
-    <row r="174" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="174" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I174" s="20"/>
       <c r="J174" s="20"/>
       <c r="K174" s="20"/>
       <c r="L174" s="22"/>
       <c r="M174" s="22"/>
     </row>
-    <row r="175" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="175" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I175" s="20"/>
       <c r="J175" s="20"/>
       <c r="K175" s="20"/>
       <c r="L175" s="22"/>
       <c r="M175" s="22"/>
     </row>
-    <row r="176" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="176" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I176" s="20"/>
       <c r="J176" s="20"/>
       <c r="K176" s="20"/>
       <c r="L176" s="22"/>
       <c r="M176" s="22"/>
     </row>
-    <row r="177" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="177" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I177" s="20"/>
       <c r="J177" s="20"/>
       <c r="K177" s="20"/>
       <c r="L177" s="22"/>
       <c r="M177" s="22"/>
     </row>
-    <row r="178" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="178" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I178" s="20"/>
       <c r="J178" s="20"/>
       <c r="K178" s="20"/>
       <c r="L178" s="22"/>
       <c r="M178" s="22"/>
     </row>
-    <row r="179" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="179" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I179" s="20"/>
       <c r="J179" s="20"/>
       <c r="K179" s="20"/>
       <c r="L179" s="22"/>
       <c r="M179" s="22"/>
     </row>
-    <row r="180" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="180" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I180" s="20"/>
       <c r="J180" s="20"/>
       <c r="K180" s="20"/>
       <c r="L180" s="22"/>
       <c r="M180" s="22"/>
     </row>
-    <row r="181" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="181" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I181" s="20"/>
       <c r="J181" s="20"/>
       <c r="K181" s="20"/>
       <c r="L181" s="22"/>
       <c r="M181" s="22"/>
     </row>
-    <row r="182" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="182" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I182" s="20"/>
       <c r="J182" s="20"/>
       <c r="K182" s="20"/>
       <c r="L182" s="22"/>
       <c r="M182" s="22"/>
     </row>
-    <row r="183" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="183" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I183" s="20"/>
       <c r="J183" s="20"/>
       <c r="K183" s="20"/>
       <c r="L183" s="22"/>
       <c r="M183" s="22"/>
     </row>
-    <row r="184" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="184" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I184" s="20"/>
       <c r="J184" s="20"/>
       <c r="K184" s="20"/>
       <c r="L184" s="22"/>
       <c r="M184" s="22"/>
     </row>
-    <row r="185" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="185" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I185" s="20"/>
       <c r="J185" s="20"/>
       <c r="K185" s="20"/>
       <c r="L185" s="22"/>
       <c r="M185" s="22"/>
     </row>
-    <row r="186" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="186" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I186" s="20"/>
       <c r="J186" s="20"/>
       <c r="K186" s="20"/>
       <c r="L186" s="22"/>
       <c r="M186" s="22"/>
     </row>
-    <row r="187" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="187" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I187" s="20"/>
       <c r="J187" s="20"/>
       <c r="K187" s="20"/>
       <c r="L187" s="22"/>
       <c r="M187" s="22"/>
     </row>
-    <row r="188" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="188" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I188" s="20"/>
       <c r="J188" s="20"/>
       <c r="K188" s="20"/>
       <c r="L188" s="22"/>
       <c r="M188" s="22"/>
     </row>
-    <row r="189" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="189" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I189" s="20"/>
       <c r="J189" s="20"/>
       <c r="K189" s="20"/>
       <c r="L189" s="22"/>
       <c r="M189" s="22"/>
     </row>
-    <row r="190" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="190" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I190" s="20"/>
       <c r="J190" s="20"/>
       <c r="K190" s="20"/>
       <c r="L190" s="22"/>
       <c r="M190" s="22"/>
     </row>
-    <row r="191" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="191" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I191" s="20"/>
       <c r="J191" s="20"/>
       <c r="K191" s="20"/>
       <c r="L191" s="22"/>
       <c r="M191" s="22"/>
     </row>
-    <row r="192" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="192" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I192" s="20"/>
       <c r="J192" s="20"/>
       <c r="K192" s="20"/>
       <c r="L192" s="22"/>
       <c r="M192" s="22"/>
     </row>
-    <row r="193" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="193" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I193" s="20"/>
       <c r="J193" s="20"/>
       <c r="K193" s="20"/>
       <c r="L193" s="22"/>
       <c r="M193" s="22"/>
     </row>
-    <row r="194" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="194" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I194" s="20"/>
       <c r="J194" s="20"/>
       <c r="K194" s="20"/>
       <c r="L194" s="22"/>
       <c r="M194" s="22"/>
     </row>
-    <row r="195" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="195" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I195" s="20"/>
       <c r="J195" s="20"/>
       <c r="K195" s="20"/>
       <c r="L195" s="22"/>
       <c r="M195" s="22"/>
     </row>
-    <row r="196" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="196" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I196" s="20"/>
       <c r="J196" s="20"/>
       <c r="K196" s="20"/>
       <c r="L196" s="22"/>
       <c r="M196" s="22"/>
     </row>
-    <row r="197" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="197" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I197" s="20"/>
       <c r="J197" s="20"/>
       <c r="K197" s="20"/>
       <c r="L197" s="22"/>
       <c r="M197" s="22"/>
     </row>
-    <row r="198" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="198" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I198" s="20"/>
       <c r="J198" s="20"/>
       <c r="K198" s="20"/>
       <c r="L198" s="22"/>
       <c r="M198" s="22"/>
     </row>
-    <row r="199" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="199" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I199" s="20"/>
       <c r="J199" s="20"/>
       <c r="K199" s="20"/>
       <c r="L199" s="22"/>
       <c r="M199" s="22"/>
     </row>
-    <row r="200" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="200" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I200" s="20"/>
       <c r="J200" s="20"/>
       <c r="K200" s="20"/>
       <c r="L200" s="22"/>
       <c r="M200" s="22"/>
     </row>
-    <row r="201" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="201" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I201" s="20"/>
       <c r="J201" s="20"/>
       <c r="K201" s="20"/>
       <c r="L201" s="22"/>
       <c r="M201" s="22"/>
     </row>
-    <row r="202" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="202" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I202" s="20"/>
       <c r="J202" s="20"/>
       <c r="K202" s="20"/>
       <c r="L202" s="22"/>
       <c r="M202" s="22"/>
     </row>
-    <row r="203" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="203" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I203" s="20"/>
       <c r="J203" s="20"/>
       <c r="K203" s="20"/>
       <c r="L203" s="22"/>
       <c r="M203" s="22"/>
     </row>
-    <row r="204" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="204" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I204" s="20"/>
       <c r="J204" s="20"/>
       <c r="K204" s="20"/>
       <c r="L204" s="22"/>
       <c r="M204" s="22"/>
     </row>
-    <row r="205" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="205" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I205" s="20"/>
       <c r="J205" s="20"/>
       <c r="K205" s="20"/>
       <c r="L205" s="22"/>
       <c r="M205" s="22"/>
     </row>
-    <row r="206" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="206" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I206" s="20"/>
       <c r="J206" s="20"/>
       <c r="K206" s="20"/>
       <c r="L206" s="22"/>
       <c r="M206" s="22"/>
     </row>
-    <row r="207" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="207" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I207" s="20"/>
       <c r="J207" s="20"/>
       <c r="K207" s="20"/>
       <c r="L207" s="22"/>
       <c r="M207" s="22"/>
     </row>
-    <row r="208" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="208" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I208" s="20"/>
       <c r="J208" s="20"/>
       <c r="K208" s="20"/>
       <c r="L208" s="22"/>
       <c r="M208" s="22"/>
     </row>
-    <row r="209" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="209" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I209" s="20"/>
       <c r="J209" s="20"/>
       <c r="K209" s="20"/>
       <c r="L209" s="22"/>
       <c r="M209" s="22"/>
     </row>
-    <row r="210" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="210" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I210" s="20"/>
       <c r="J210" s="20"/>
       <c r="K210" s="20"/>
       <c r="L210" s="22"/>
       <c r="M210" s="22"/>
     </row>
-    <row r="211" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="211" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I211" s="20"/>
       <c r="J211" s="20"/>
       <c r="K211" s="20"/>
       <c r="L211" s="22"/>
       <c r="M211" s="22"/>
     </row>
-    <row r="212" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="212" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I212" s="20"/>
       <c r="J212" s="20"/>
       <c r="K212" s="20"/>
       <c r="L212" s="22"/>
       <c r="M212" s="22"/>
     </row>
-    <row r="213" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="213" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I213" s="20"/>
       <c r="J213" s="20"/>
       <c r="K213" s="20"/>
       <c r="L213" s="22"/>
       <c r="M213" s="22"/>
     </row>
-    <row r="214" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="214" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I214" s="20"/>
       <c r="J214" s="20"/>
       <c r="K214" s="20"/>
       <c r="L214" s="22"/>
       <c r="M214" s="22"/>
     </row>
-    <row r="215" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="215" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I215" s="20"/>
       <c r="J215" s="20"/>
       <c r="K215" s="20"/>
       <c r="L215" s="22"/>
       <c r="M215" s="22"/>
     </row>
-    <row r="216" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="216" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I216" s="20"/>
       <c r="J216" s="20"/>
       <c r="K216" s="20"/>
       <c r="L216" s="22"/>
       <c r="M216" s="22"/>
     </row>
-    <row r="217" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="217" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I217" s="20"/>
       <c r="J217" s="20"/>
       <c r="K217" s="20"/>
       <c r="L217" s="22"/>
       <c r="M217" s="22"/>
     </row>
-    <row r="218" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="218" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I218" s="20"/>
       <c r="J218" s="20"/>
       <c r="K218" s="20"/>
       <c r="L218" s="22"/>
       <c r="M218" s="22"/>
     </row>
-    <row r="219" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="219" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I219" s="20"/>
       <c r="J219" s="20"/>
       <c r="K219" s="20"/>
       <c r="L219" s="22"/>
       <c r="M219" s="22"/>
     </row>
-    <row r="220" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="220" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I220" s="20"/>
       <c r="J220" s="20"/>
       <c r="K220" s="20"/>
       <c r="L220" s="22"/>
       <c r="M220" s="22"/>
     </row>
-    <row r="221" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="221" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I221" s="20"/>
       <c r="J221" s="20"/>
       <c r="K221" s="20"/>
       <c r="L221" s="22"/>
       <c r="M221" s="22"/>
     </row>
-    <row r="222" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="222" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I222" s="20"/>
       <c r="J222" s="20"/>
       <c r="K222" s="20"/>
       <c r="L222" s="22"/>
       <c r="M222" s="22"/>
     </row>
-    <row r="223" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="223" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I223" s="20"/>
       <c r="J223" s="20"/>
       <c r="K223" s="20"/>
       <c r="L223" s="22"/>
       <c r="M223" s="22"/>
     </row>
-    <row r="224" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="224" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I224" s="20"/>
       <c r="J224" s="20"/>
       <c r="K224" s="20"/>
       <c r="L224" s="22"/>
       <c r="M224" s="22"/>
     </row>
-    <row r="225" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="225" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I225" s="20"/>
       <c r="J225" s="20"/>
       <c r="K225" s="20"/>
       <c r="L225" s="22"/>
       <c r="M225" s="22"/>
     </row>
-    <row r="226" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="226" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I226" s="20"/>
       <c r="J226" s="20"/>
       <c r="K226" s="20"/>
       <c r="L226" s="22"/>
       <c r="M226" s="22"/>
     </row>
-    <row r="227" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="227" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I227" s="20"/>
       <c r="J227" s="20"/>
       <c r="K227" s="20"/>
       <c r="L227" s="22"/>
       <c r="M227" s="22"/>
     </row>
-    <row r="228" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="228" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I228" s="20"/>
       <c r="J228" s="20"/>
       <c r="K228" s="20"/>
       <c r="L228" s="22"/>
       <c r="M228" s="22"/>
     </row>
-    <row r="229" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="229" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I229" s="20"/>
       <c r="J229" s="20"/>
       <c r="K229" s="20"/>
       <c r="L229" s="22"/>
       <c r="M229" s="22"/>
     </row>
-    <row r="230" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="230" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I230" s="20"/>
       <c r="J230" s="20"/>
       <c r="K230" s="20"/>
       <c r="L230" s="22"/>
       <c r="M230" s="22"/>
     </row>
-    <row r="231" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="231" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I231" s="20"/>
       <c r="J231" s="20"/>
       <c r="K231" s="20"/>
       <c r="L231" s="22"/>
       <c r="M231" s="22"/>
     </row>
-    <row r="232" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="232" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I232" s="20"/>
       <c r="J232" s="20"/>
       <c r="K232" s="20"/>
       <c r="L232" s="22"/>
       <c r="M232" s="22"/>
     </row>
-    <row r="233" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="233" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I233" s="20"/>
       <c r="J233" s="20"/>
       <c r="K233" s="20"/>
       <c r="L233" s="22"/>
       <c r="M233" s="22"/>
     </row>
-    <row r="234" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="234" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I234" s="20"/>
       <c r="J234" s="20"/>
       <c r="K234" s="20"/>
     </row>
-    <row r="235" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="235" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I235" s="20"/>
       <c r="J235" s="20"/>
       <c r="K235" s="20"/>
     </row>
-    <row r="236" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="236" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I236" s="20"/>
       <c r="J236" s="20"/>
       <c r="K236" s="20"/>
     </row>
-    <row r="237" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="237" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I237" s="20"/>
       <c r="J237" s="20"/>
       <c r="K237" s="20"/>
     </row>
-    <row r="238" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="238" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I238" s="20"/>
       <c r="J238" s="20"/>
       <c r="K238" s="20"/>
     </row>
-    <row r="239" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="239" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I239" s="20"/>
       <c r="J239" s="20"/>
       <c r="K239" s="20"/>
     </row>
-    <row r="240" spans="9:13" x14ac:dyDescent="0.45">
+    <row r="240" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I240" s="20"/>
       <c r="J240" s="20"/>
       <c r="K240" s="20"/>
     </row>
-    <row r="241" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="241" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I241" s="20"/>
       <c r="J241" s="20"/>
       <c r="K241" s="20"/>
     </row>
-    <row r="242" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="242" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I242" s="20"/>
       <c r="J242" s="20"/>
       <c r="K242" s="20"/>
     </row>
-    <row r="243" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="243" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I243" s="20"/>
       <c r="J243" s="20"/>
       <c r="K243" s="20"/>
     </row>
-    <row r="244" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="244" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I244" s="20"/>
       <c r="J244" s="20"/>
       <c r="K244" s="20"/>
     </row>
-    <row r="245" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="245" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I245" s="20"/>
       <c r="J245" s="20"/>
       <c r="K245" s="20"/>
     </row>
-    <row r="246" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="246" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I246" s="20"/>
       <c r="J246" s="20"/>
       <c r="K246" s="20"/>
     </row>
-    <row r="247" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="247" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I247" s="20"/>
       <c r="J247" s="20"/>
       <c r="K247" s="20"/>
     </row>
-    <row r="248" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="248" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I248" s="20"/>
       <c r="J248" s="20"/>
       <c r="K248" s="20"/>
     </row>
-    <row r="249" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="249" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I249" s="20"/>
       <c r="J249" s="20"/>
       <c r="K249" s="20"/>
     </row>
-    <row r="250" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="250" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I250" s="20"/>
       <c r="J250" s="20"/>
       <c r="K250" s="20"/>
     </row>
-    <row r="251" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="251" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I251" s="20"/>
       <c r="J251" s="20"/>
       <c r="K251" s="20"/>
     </row>
-    <row r="252" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="252" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I252" s="20"/>
       <c r="J252" s="20"/>
       <c r="K252" s="20"/>
     </row>
-    <row r="253" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="253" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I253" s="20"/>
       <c r="J253" s="20"/>
       <c r="K253" s="20"/>
     </row>
-    <row r="254" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="254" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I254" s="20"/>
       <c r="J254" s="20"/>
       <c r="K254" s="20"/>
     </row>
-    <row r="255" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="255" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I255" s="20"/>
       <c r="J255" s="20"/>
       <c r="K255" s="20"/>
     </row>
-    <row r="256" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="256" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I256" s="20"/>
       <c r="J256" s="20"/>
       <c r="K256" s="20"/>
     </row>
-    <row r="257" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="257" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I257" s="20"/>
       <c r="J257" s="20"/>
       <c r="K257" s="20"/>
     </row>
-    <row r="258" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="258" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I258" s="20"/>
       <c r="J258" s="20"/>
       <c r="K258" s="20"/>
     </row>
-    <row r="259" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="259" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I259" s="20"/>
       <c r="J259" s="20"/>
       <c r="K259" s="20"/>
     </row>
-    <row r="260" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="260" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I260" s="20"/>
       <c r="J260" s="20"/>
       <c r="K260" s="20"/>
     </row>
-    <row r="261" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="261" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I261" s="20"/>
       <c r="J261" s="20"/>
       <c r="K261" s="20"/>
     </row>
-    <row r="262" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="262" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I262" s="20"/>
       <c r="J262" s="20"/>
       <c r="K262" s="20"/>
     </row>
-    <row r="263" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="263" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I263" s="20"/>
       <c r="J263" s="20"/>
       <c r="K263" s="20"/>
     </row>
-    <row r="264" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="264" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I264" s="20"/>
       <c r="J264" s="20"/>
       <c r="K264" s="20"/>
     </row>
-    <row r="265" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="265" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I265" s="20"/>
       <c r="J265" s="20"/>
       <c r="K265" s="20"/>
     </row>
-    <row r="266" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="266" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I266" s="20"/>
       <c r="J266" s="20"/>
       <c r="K266" s="20"/>
     </row>
-    <row r="267" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="267" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I267" s="20"/>
       <c r="J267" s="20"/>
       <c r="K267" s="20"/>
     </row>
-    <row r="268" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="268" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I268" s="20"/>
       <c r="J268" s="20"/>
       <c r="K268" s="20"/>
     </row>
-    <row r="269" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="269" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I269" s="20"/>
       <c r="J269" s="20"/>
       <c r="K269" s="20"/>
     </row>
-    <row r="270" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="270" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I270" s="20"/>
       <c r="J270" s="20"/>
       <c r="K270" s="20"/>
     </row>
-    <row r="271" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="271" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I271" s="20"/>
       <c r="J271" s="20"/>
       <c r="K271" s="20"/>
     </row>
-    <row r="272" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="272" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I272" s="20"/>
       <c r="J272" s="20"/>
       <c r="K272" s="20"/>
     </row>
-    <row r="273" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="273" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I273" s="20"/>
       <c r="J273" s="20"/>
       <c r="K273" s="20"/>
     </row>
-    <row r="274" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="274" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I274" s="20"/>
       <c r="J274" s="20"/>
       <c r="K274" s="20"/>
     </row>
-    <row r="275" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="275" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I275" s="20"/>
       <c r="J275" s="20"/>
       <c r="K275" s="20"/>
     </row>
-    <row r="276" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="276" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I276" s="20"/>
       <c r="J276" s="20"/>
       <c r="K276" s="20"/>
     </row>
-    <row r="277" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="277" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I277" s="20"/>
       <c r="J277" s="20"/>
       <c r="K277" s="20"/>
     </row>
-    <row r="278" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="278" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I278" s="20"/>
       <c r="J278" s="20"/>
       <c r="K278" s="20"/>
     </row>
-    <row r="279" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="279" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I279" s="20"/>
       <c r="J279" s="20"/>
       <c r="K279" s="20"/>
     </row>
-    <row r="280" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="280" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I280" s="20"/>
       <c r="J280" s="20"/>
       <c r="K280" s="20"/>
     </row>
-    <row r="281" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="281" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I281" s="20"/>
       <c r="J281" s="20"/>
       <c r="K281" s="20"/>
     </row>
-    <row r="282" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="282" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I282" s="20"/>
       <c r="J282" s="20"/>
       <c r="K282" s="20"/>
     </row>
-    <row r="283" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="283" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I283" s="20"/>
       <c r="J283" s="20"/>
       <c r="K283" s="20"/>
     </row>
-    <row r="284" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="284" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I284" s="20"/>
       <c r="J284" s="20"/>
       <c r="K284" s="20"/>
     </row>
-    <row r="285" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="285" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I285" s="20"/>
       <c r="J285" s="20"/>
       <c r="K285" s="20"/>
     </row>
-    <row r="286" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="286" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I286" s="20"/>
       <c r="J286" s="20"/>
       <c r="K286" s="20"/>
     </row>
-    <row r="287" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="287" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I287" s="20"/>
       <c r="J287" s="20"/>
       <c r="K287" s="20"/>
     </row>
-    <row r="288" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="288" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I288" s="20"/>
       <c r="J288" s="20"/>
       <c r="K288" s="20"/>
     </row>
-    <row r="289" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="289" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I289" s="20"/>
       <c r="J289" s="20"/>
       <c r="K289" s="20"/>
     </row>
-    <row r="290" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="290" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I290" s="20"/>
       <c r="J290" s="20"/>
       <c r="K290" s="20"/>
     </row>
-    <row r="291" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="291" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I291" s="20"/>
       <c r="J291" s="20"/>
       <c r="K291" s="20"/>
     </row>
-    <row r="292" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="292" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I292" s="20"/>
       <c r="J292" s="20"/>
       <c r="K292" s="20"/>
     </row>
-    <row r="293" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="293" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I293" s="20"/>
       <c r="J293" s="20"/>
       <c r="K293" s="20"/>
     </row>
-    <row r="294" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="294" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I294" s="20"/>
       <c r="J294" s="20"/>
       <c r="K294" s="20"/>
     </row>
-    <row r="295" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="295" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I295" s="20"/>
       <c r="J295" s="20"/>
       <c r="K295" s="20"/>
     </row>
-    <row r="296" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="296" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I296" s="20"/>
       <c r="J296" s="20"/>
       <c r="K296" s="20"/>
     </row>
-    <row r="297" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="297" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I297" s="20"/>
       <c r="J297" s="20"/>
       <c r="K297" s="20"/>
     </row>
-    <row r="298" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="298" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I298" s="20"/>
       <c r="J298" s="20"/>
       <c r="K298" s="20"/>
     </row>
-    <row r="299" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="299" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I299" s="20"/>
       <c r="J299" s="20"/>
       <c r="K299" s="20"/>
     </row>
-    <row r="300" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="300" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I300" s="20"/>
       <c r="J300" s="20"/>
       <c r="K300" s="20"/>
     </row>
-    <row r="301" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="301" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I301" s="20"/>
       <c r="J301" s="20"/>
       <c r="K301" s="20"/>
     </row>
-    <row r="302" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="302" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I302" s="20"/>
       <c r="J302" s="20"/>
       <c r="K302" s="20"/>
     </row>
-    <row r="303" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="303" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I303" s="20"/>
       <c r="J303" s="20"/>
       <c r="K303" s="20"/>
     </row>
-    <row r="304" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="304" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I304" s="20"/>
       <c r="J304" s="20"/>
       <c r="K304" s="20"/>
     </row>
-    <row r="305" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="305" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I305" s="20"/>
       <c r="J305" s="20"/>
       <c r="K305" s="20"/>
     </row>
-    <row r="306" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="306" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I306" s="20"/>
       <c r="J306" s="20"/>
       <c r="K306" s="20"/>
     </row>
-    <row r="307" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="307" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I307" s="20"/>
       <c r="J307" s="20"/>
       <c r="K307" s="20"/>
     </row>
-    <row r="308" spans="9:11" x14ac:dyDescent="0.45">
+    <row r="308" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I308" s="20"/>
       <c r="J308" s="20"/>
       <c r="K308" s="20"/>
@@ -30505,25 +30515,25 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L19" sqref="L19"/>
-      <selection pane="bottomLeft" activeCell="R36" sqref="R36"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.3984375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30546,7 +30556,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>43</v>
@@ -30571,7 +30581,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -30596,7 +30606,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30619,6 +30629,16 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
+    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="R24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30639,17 +30659,17 @@
       <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.3984375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30672,7 +30692,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>38</v>
@@ -30697,7 +30717,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>28</v>
@@ -30724,7 +30744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30767,17 +30787,17 @@
       <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.3984375" style="1"/>
-    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.3984375" style="1"/>
+    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30800,7 +30820,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>39</v>
@@ -30825,7 +30845,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>42</v>
@@ -30852,7 +30872,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30875,7 +30895,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
-    <row r="45" ht="57.75" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="45" ht="57.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30895,12 +30915,12 @@
       <selection pane="bottomLeft" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.73046875" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30923,7 +30943,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>27</v>
@@ -30948,7 +30968,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="str">
         <f>Übersicht!B3</f>
@@ -30976,7 +30996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>

</xml_diff>

<commit_message>
Update 8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
added Kontrollabfrage Direktaufgaben
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
+++ b/8. Harmonising standards/01_Project organisation/01_Project Workflow/Project WorkFlow 1.0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B071EC-79FD-4D54-8CC7-6405E11EB45A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCAC50C-ECC4-4DF2-92F9-ABC66CDBEC9C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="4425" tabRatio="837" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Abgeschlossen</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Installation läßt sich nicht einfach DF und SXI zuordnen - wie umgehen ?</t>
+  </si>
+  <si>
+    <t>Direktaufgaben dürfen nicht älter als 3 Monate sein, sonst wurde meist</t>
+  </si>
+  <si>
+    <t>die Abrechnung vergessen -&gt; Auswertung !</t>
   </si>
 </sst>
 </file>
@@ -28026,17 +28032,17 @@
       <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -28059,7 +28065,7 @@
       <c r="T1" s="11"/>
       <c r="U1" s="11"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>25</v>
@@ -28084,7 +28090,7 @@
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>28</v>
@@ -28111,7 +28117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -28134,12 +28140,12 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
@@ -28147,10 +28153,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
@@ -28158,10 +28164,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="s">
         <v>39</v>
       </c>
@@ -28169,17 +28175,17 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="B16" s="8"/>
       <c r="E16" s="25"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="8"/>
       <c r="E17" s="25"/>
     </row>
@@ -28209,22 +28215,22 @@
       <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" outlineLevelRow="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="1" customWidth="1"/>
-    <col min="5" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="11" width="15.7109375" style="9" customWidth="1"/>
-    <col min="12" max="12" width="29.28515625" style="9" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" style="9"/>
-    <col min="14" max="14" width="50.7109375" style="9" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.73046875" style="1" customWidth="1"/>
+    <col min="5" max="7" width="11.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="15.73046875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="29.265625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="11.3984375" style="9"/>
+    <col min="14" max="14" width="50.73046875" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -28240,7 +28246,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>26</v>
@@ -28258,7 +28264,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="str">
         <f>Übersicht!B3</f>
@@ -28279,7 +28285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -28295,7 +28301,7 @@
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I6" s="15" t="s">
         <v>6</v>
       </c>
@@ -28309,7 +28315,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="35"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I7" s="13" t="s">
         <v>1</v>
       </c>
@@ -28329,7 +28335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -28337,7 +28343,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="35"/>
     </row>
-    <row r="9" spans="1:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" collapsed="1" x14ac:dyDescent="0.45">
       <c r="B9" s="31" t="s">
         <v>0</v>
       </c>
@@ -28354,7 +28360,7 @@
       <c r="M9" s="33"/>
       <c r="N9" s="36"/>
     </row>
-    <row r="10" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -28362,7 +28368,7 @@
       <c r="M10" s="21"/>
       <c r="N10" s="35"/>
     </row>
-    <row r="11" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B11" s="26" t="s">
         <v>23</v>
       </c>
@@ -28381,7 +28387,7 @@
       <c r="M11" s="30"/>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="4" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B12" s="40"/>
       <c r="H12" s="41"/>
       <c r="I12" s="42"/>
@@ -28391,7 +28397,7 @@
       <c r="M12" s="43"/>
       <c r="N12" s="44"/>
     </row>
-    <row r="13" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B13" s="17">
         <v>1</v>
       </c>
@@ -28416,7 +28422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B14" s="16" t="s">
         <v>9</v>
       </c>
@@ -28430,7 +28436,7 @@
       <c r="M14" s="21"/>
       <c r="N14" s="35"/>
     </row>
-    <row r="15" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C15" s="18" t="s">
         <v>14</v>
       </c>
@@ -28441,7 +28447,7 @@
       <c r="M15" s="21"/>
       <c r="N15" s="35"/>
     </row>
-    <row r="16" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
       <c r="K16" s="19"/>
@@ -28449,7 +28455,7 @@
       <c r="M16" s="21"/>
       <c r="N16" s="35"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
       <c r="K17" s="19"/>
@@ -28457,7 +28463,7 @@
       <c r="M17" s="21"/>
       <c r="N17" s="35"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B18" s="31" t="s">
         <v>21</v>
       </c>
@@ -28474,7 +28480,7 @@
       <c r="M18" s="33"/>
       <c r="N18" s="36"/>
     </row>
-    <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
       <c r="K19" s="19"/>
@@ -28482,7 +28488,7 @@
       <c r="M19" s="21"/>
       <c r="N19" s="35"/>
     </row>
-    <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B20" s="26" t="s">
         <v>29</v>
       </c>
@@ -28501,7 +28507,7 @@
       <c r="M20" s="30"/>
       <c r="N20" s="37"/>
     </row>
-    <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I21" s="19"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
@@ -28509,7 +28515,7 @@
       <c r="M21" s="21"/>
       <c r="N21" s="35"/>
     </row>
-    <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B22" s="17">
         <v>1</v>
       </c>
@@ -28530,7 +28536,7 @@
       <c r="M22" s="21"/>
       <c r="N22" s="38"/>
     </row>
-    <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B23" s="16" t="s">
         <v>30</v>
       </c>
@@ -28544,7 +28550,7 @@
       <c r="M23" s="21"/>
       <c r="N23" s="38"/>
     </row>
-    <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C24" s="18" t="s">
         <v>35</v>
       </c>
@@ -28555,7 +28561,7 @@
       <c r="M24" s="21"/>
       <c r="N24" s="35"/>
     </row>
-    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I25" s="19"/>
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
@@ -28563,7 +28569,7 @@
       <c r="M25" s="21"/>
       <c r="N25" s="35"/>
     </row>
-    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B26" s="17">
         <v>2</v>
       </c>
@@ -28584,7 +28590,7 @@
       <c r="M26" s="21"/>
       <c r="N26" s="38"/>
     </row>
-    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B27" s="16" t="s">
         <v>32</v>
       </c>
@@ -28598,7 +28604,7 @@
       <c r="M27" s="21"/>
       <c r="N27" s="38"/>
     </row>
-    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C28" s="18" t="s">
         <v>37</v>
       </c>
@@ -28609,7 +28615,7 @@
       <c r="M28" s="21"/>
       <c r="N28" s="35"/>
     </row>
-    <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C29" s="18"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -28618,7 +28624,7 @@
       <c r="M29" s="21"/>
       <c r="N29" s="35"/>
     </row>
-    <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C30" s="18"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -28627,7 +28633,7 @@
       <c r="M30" s="21"/>
       <c r="N30" s="35"/>
     </row>
-    <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C31" s="18"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -28636,7 +28642,7 @@
       <c r="M31" s="21"/>
       <c r="N31" s="35"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.45">
       <c r="C32" s="18"/>
       <c r="I32" s="19"/>
       <c r="J32" s="19"/>
@@ -28645,7 +28651,7 @@
       <c r="M32" s="21"/>
       <c r="N32" s="35"/>
     </row>
-    <row r="33" spans="2:14" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" collapsed="1" x14ac:dyDescent="0.45">
       <c r="B33" s="31" t="s">
         <v>18</v>
       </c>
@@ -28662,7 +28668,7 @@
       <c r="M33" s="33"/>
       <c r="N33" s="36"/>
     </row>
-    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
       <c r="K34" s="19"/>
@@ -28670,7 +28676,7 @@
       <c r="M34" s="21"/>
       <c r="N34" s="35"/>
     </row>
-    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B35" s="17" t="s">
         <v>10</v>
       </c>
@@ -28697,7 +28703,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="B36" s="16"/>
       <c r="C36" s="18" t="s">
         <v>16</v>
@@ -28709,7 +28715,7 @@
       <c r="M36" s="21"/>
       <c r="N36" s="38"/>
     </row>
-    <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C37" s="18" t="s">
         <v>16</v>
       </c>
@@ -28720,7 +28726,7 @@
       <c r="M37" s="21"/>
       <c r="N37" s="35"/>
     </row>
-    <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C38" s="18" t="s">
         <v>16</v>
       </c>
@@ -28731,7 +28737,7 @@
       <c r="M38" s="21"/>
       <c r="N38" s="35"/>
     </row>
-    <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="C39" s="18" t="s">
         <v>16</v>
       </c>
@@ -28742,7 +28748,7 @@
       <c r="M39" s="21"/>
       <c r="N39" s="35"/>
     </row>
-    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I40" s="19"/>
       <c r="J40" s="19"/>
       <c r="K40" s="19"/>
@@ -28750,7 +28756,7 @@
       <c r="M40" s="21"/>
       <c r="N40" s="35"/>
     </row>
-    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I41" s="19"/>
       <c r="J41" s="19"/>
       <c r="K41" s="19"/>
@@ -28758,7 +28764,7 @@
       <c r="M41" s="21"/>
       <c r="N41" s="35"/>
     </row>
-    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.45">
       <c r="I42" s="19"/>
       <c r="J42" s="19"/>
       <c r="K42" s="19"/>
@@ -28766,7 +28772,7 @@
       <c r="M42" s="21"/>
       <c r="N42" s="35"/>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I43" s="20"/>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
@@ -28774,1707 +28780,1707 @@
       <c r="M43" s="22"/>
       <c r="N43" s="39"/>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I44" s="20"/>
       <c r="J44" s="20"/>
       <c r="K44" s="20"/>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I45" s="20"/>
       <c r="J45" s="20"/>
       <c r="K45" s="20"/>
       <c r="L45" s="22"/>
       <c r="M45" s="22"/>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I46" s="20"/>
       <c r="J46" s="20"/>
       <c r="K46" s="20"/>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I47" s="20"/>
       <c r="J47" s="20"/>
       <c r="K47" s="20"/>
       <c r="L47" s="22"/>
       <c r="M47" s="22"/>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.45">
       <c r="I48" s="20"/>
       <c r="J48" s="20"/>
       <c r="K48" s="20"/>
       <c r="L48" s="22"/>
       <c r="M48" s="22"/>
     </row>
-    <row r="49" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I49" s="20"/>
       <c r="J49" s="20"/>
       <c r="K49" s="20"/>
       <c r="L49" s="22"/>
       <c r="M49" s="22"/>
     </row>
-    <row r="50" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I50" s="20"/>
       <c r="J50" s="20"/>
       <c r="K50" s="20"/>
       <c r="L50" s="22"/>
       <c r="M50" s="22"/>
     </row>
-    <row r="51" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I51" s="20"/>
       <c r="J51" s="20"/>
       <c r="K51" s="20"/>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
     </row>
-    <row r="52" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I52" s="20"/>
       <c r="J52" s="20"/>
       <c r="K52" s="20"/>
       <c r="L52" s="22"/>
       <c r="M52" s="22"/>
     </row>
-    <row r="53" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I53" s="20"/>
       <c r="J53" s="20"/>
       <c r="K53" s="20"/>
       <c r="L53" s="22"/>
       <c r="M53" s="22"/>
     </row>
-    <row r="54" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I54" s="20"/>
       <c r="J54" s="20"/>
       <c r="K54" s="20"/>
       <c r="L54" s="22"/>
       <c r="M54" s="22"/>
     </row>
-    <row r="55" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I55" s="20"/>
       <c r="J55" s="20"/>
       <c r="K55" s="20"/>
       <c r="L55" s="22"/>
       <c r="M55" s="22"/>
     </row>
-    <row r="56" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I56" s="20"/>
       <c r="J56" s="20"/>
       <c r="K56" s="20"/>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
     </row>
-    <row r="57" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I57" s="20"/>
       <c r="J57" s="20"/>
       <c r="K57" s="20"/>
       <c r="L57" s="22"/>
       <c r="M57" s="22"/>
     </row>
-    <row r="58" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I58" s="20"/>
       <c r="J58" s="20"/>
       <c r="K58" s="20"/>
       <c r="L58" s="22"/>
       <c r="M58" s="22"/>
     </row>
-    <row r="59" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I59" s="20"/>
       <c r="J59" s="20"/>
       <c r="K59" s="20"/>
       <c r="L59" s="22"/>
       <c r="M59" s="22"/>
     </row>
-    <row r="60" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I60" s="20"/>
       <c r="J60" s="20"/>
       <c r="K60" s="20"/>
       <c r="L60" s="22"/>
       <c r="M60" s="22"/>
     </row>
-    <row r="61" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I61" s="20"/>
       <c r="J61" s="20"/>
       <c r="K61" s="20"/>
       <c r="L61" s="22"/>
       <c r="M61" s="22"/>
     </row>
-    <row r="62" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I62" s="20"/>
       <c r="J62" s="20"/>
       <c r="K62" s="20"/>
       <c r="L62" s="22"/>
       <c r="M62" s="22"/>
     </row>
-    <row r="63" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I63" s="20"/>
       <c r="J63" s="20"/>
       <c r="K63" s="20"/>
       <c r="L63" s="22"/>
       <c r="M63" s="22"/>
     </row>
-    <row r="64" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I64" s="20"/>
       <c r="J64" s="20"/>
       <c r="K64" s="20"/>
       <c r="L64" s="22"/>
       <c r="M64" s="22"/>
     </row>
-    <row r="65" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I65" s="20"/>
       <c r="J65" s="20"/>
       <c r="K65" s="20"/>
       <c r="L65" s="22"/>
       <c r="M65" s="22"/>
     </row>
-    <row r="66" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I66" s="20"/>
       <c r="J66" s="20"/>
       <c r="K66" s="20"/>
       <c r="L66" s="22"/>
       <c r="M66" s="22"/>
     </row>
-    <row r="67" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I67" s="20"/>
       <c r="J67" s="20"/>
       <c r="K67" s="20"/>
       <c r="L67" s="22"/>
       <c r="M67" s="22"/>
     </row>
-    <row r="68" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I68" s="20"/>
       <c r="J68" s="20"/>
       <c r="K68" s="20"/>
       <c r="L68" s="22"/>
       <c r="M68" s="22"/>
     </row>
-    <row r="69" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I69" s="20"/>
       <c r="J69" s="20"/>
       <c r="K69" s="20"/>
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
     </row>
-    <row r="70" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I70" s="20"/>
       <c r="J70" s="20"/>
       <c r="K70" s="20"/>
       <c r="L70" s="22"/>
       <c r="M70" s="22"/>
     </row>
-    <row r="71" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I71" s="20"/>
       <c r="J71" s="20"/>
       <c r="K71" s="20"/>
       <c r="L71" s="22"/>
       <c r="M71" s="22"/>
     </row>
-    <row r="72" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I72" s="20"/>
       <c r="J72" s="20"/>
       <c r="K72" s="20"/>
       <c r="L72" s="22"/>
       <c r="M72" s="22"/>
     </row>
-    <row r="73" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I73" s="20"/>
       <c r="J73" s="20"/>
       <c r="K73" s="20"/>
       <c r="L73" s="22"/>
       <c r="M73" s="22"/>
     </row>
-    <row r="74" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I74" s="20"/>
       <c r="J74" s="20"/>
       <c r="K74" s="20"/>
       <c r="L74" s="22"/>
       <c r="M74" s="22"/>
     </row>
-    <row r="75" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I75" s="20"/>
       <c r="J75" s="20"/>
       <c r="K75" s="20"/>
       <c r="L75" s="22"/>
       <c r="M75" s="22"/>
     </row>
-    <row r="76" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I76" s="20"/>
       <c r="J76" s="20"/>
       <c r="K76" s="20"/>
       <c r="L76" s="22"/>
       <c r="M76" s="22"/>
     </row>
-    <row r="77" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I77" s="20"/>
       <c r="J77" s="20"/>
       <c r="K77" s="20"/>
       <c r="L77" s="22"/>
       <c r="M77" s="22"/>
     </row>
-    <row r="78" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I78" s="20"/>
       <c r="J78" s="20"/>
       <c r="K78" s="20"/>
       <c r="L78" s="22"/>
       <c r="M78" s="22"/>
     </row>
-    <row r="79" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I79" s="20"/>
       <c r="J79" s="20"/>
       <c r="K79" s="20"/>
       <c r="L79" s="22"/>
       <c r="M79" s="22"/>
     </row>
-    <row r="80" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I80" s="20"/>
       <c r="J80" s="20"/>
       <c r="K80" s="20"/>
       <c r="L80" s="22"/>
       <c r="M80" s="22"/>
     </row>
-    <row r="81" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I81" s="20"/>
       <c r="J81" s="20"/>
       <c r="K81" s="20"/>
       <c r="L81" s="22"/>
       <c r="M81" s="22"/>
     </row>
-    <row r="82" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I82" s="20"/>
       <c r="J82" s="20"/>
       <c r="K82" s="20"/>
       <c r="L82" s="22"/>
       <c r="M82" s="22"/>
     </row>
-    <row r="83" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I83" s="20"/>
       <c r="J83" s="20"/>
       <c r="K83" s="20"/>
       <c r="L83" s="22"/>
       <c r="M83" s="22"/>
     </row>
-    <row r="84" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I84" s="20"/>
       <c r="J84" s="20"/>
       <c r="K84" s="20"/>
       <c r="L84" s="22"/>
       <c r="M84" s="22"/>
     </row>
-    <row r="85" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I85" s="20"/>
       <c r="J85" s="20"/>
       <c r="K85" s="20"/>
       <c r="L85" s="22"/>
       <c r="M85" s="22"/>
     </row>
-    <row r="86" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I86" s="20"/>
       <c r="J86" s="20"/>
       <c r="K86" s="20"/>
       <c r="L86" s="22"/>
       <c r="M86" s="22"/>
     </row>
-    <row r="87" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I87" s="20"/>
       <c r="J87" s="20"/>
       <c r="K87" s="20"/>
       <c r="L87" s="22"/>
       <c r="M87" s="22"/>
     </row>
-    <row r="88" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I88" s="20"/>
       <c r="J88" s="20"/>
       <c r="K88" s="20"/>
       <c r="L88" s="22"/>
       <c r="M88" s="22"/>
     </row>
-    <row r="89" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I89" s="20"/>
       <c r="J89" s="20"/>
       <c r="K89" s="20"/>
       <c r="L89" s="22"/>
       <c r="M89" s="22"/>
     </row>
-    <row r="90" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I90" s="20"/>
       <c r="J90" s="20"/>
       <c r="K90" s="20"/>
       <c r="L90" s="22"/>
       <c r="M90" s="22"/>
     </row>
-    <row r="91" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I91" s="20"/>
       <c r="J91" s="20"/>
       <c r="K91" s="20"/>
       <c r="L91" s="22"/>
       <c r="M91" s="22"/>
     </row>
-    <row r="92" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I92" s="20"/>
       <c r="J92" s="20"/>
       <c r="K92" s="20"/>
       <c r="L92" s="22"/>
       <c r="M92" s="22"/>
     </row>
-    <row r="93" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I93" s="20"/>
       <c r="J93" s="20"/>
       <c r="K93" s="20"/>
       <c r="L93" s="22"/>
       <c r="M93" s="22"/>
     </row>
-    <row r="94" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I94" s="20"/>
       <c r="J94" s="20"/>
       <c r="K94" s="20"/>
       <c r="L94" s="22"/>
       <c r="M94" s="22"/>
     </row>
-    <row r="95" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I95" s="20"/>
       <c r="J95" s="20"/>
       <c r="K95" s="20"/>
       <c r="L95" s="22"/>
       <c r="M95" s="22"/>
     </row>
-    <row r="96" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I96" s="20"/>
       <c r="J96" s="20"/>
       <c r="K96" s="20"/>
       <c r="L96" s="22"/>
       <c r="M96" s="22"/>
     </row>
-    <row r="97" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I97" s="20"/>
       <c r="J97" s="20"/>
       <c r="K97" s="20"/>
       <c r="L97" s="22"/>
       <c r="M97" s="22"/>
     </row>
-    <row r="98" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I98" s="20"/>
       <c r="J98" s="20"/>
       <c r="K98" s="20"/>
       <c r="L98" s="22"/>
       <c r="M98" s="22"/>
     </row>
-    <row r="99" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I99" s="20"/>
       <c r="J99" s="20"/>
       <c r="K99" s="20"/>
       <c r="L99" s="22"/>
       <c r="M99" s="22"/>
     </row>
-    <row r="100" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I100" s="20"/>
       <c r="J100" s="20"/>
       <c r="K100" s="20"/>
       <c r="L100" s="22"/>
       <c r="M100" s="22"/>
     </row>
-    <row r="101" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I101" s="20"/>
       <c r="J101" s="20"/>
       <c r="K101" s="20"/>
       <c r="L101" s="22"/>
       <c r="M101" s="22"/>
     </row>
-    <row r="102" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I102" s="20"/>
       <c r="J102" s="20"/>
       <c r="K102" s="20"/>
       <c r="L102" s="22"/>
       <c r="M102" s="22"/>
     </row>
-    <row r="103" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I103" s="20"/>
       <c r="J103" s="20"/>
       <c r="K103" s="20"/>
       <c r="L103" s="22"/>
       <c r="M103" s="22"/>
     </row>
-    <row r="104" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I104" s="20"/>
       <c r="J104" s="20"/>
       <c r="K104" s="20"/>
       <c r="L104" s="22"/>
       <c r="M104" s="22"/>
     </row>
-    <row r="105" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I105" s="20"/>
       <c r="J105" s="20"/>
       <c r="K105" s="20"/>
       <c r="L105" s="22"/>
       <c r="M105" s="22"/>
     </row>
-    <row r="106" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I106" s="20"/>
       <c r="J106" s="20"/>
       <c r="K106" s="20"/>
       <c r="L106" s="22"/>
       <c r="M106" s="22"/>
     </row>
-    <row r="107" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I107" s="20"/>
       <c r="J107" s="20"/>
       <c r="K107" s="20"/>
       <c r="L107" s="22"/>
       <c r="M107" s="22"/>
     </row>
-    <row r="108" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I108" s="20"/>
       <c r="J108" s="20"/>
       <c r="K108" s="20"/>
       <c r="L108" s="22"/>
       <c r="M108" s="22"/>
     </row>
-    <row r="109" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I109" s="20"/>
       <c r="J109" s="20"/>
       <c r="K109" s="20"/>
       <c r="L109" s="22"/>
       <c r="M109" s="22"/>
     </row>
-    <row r="110" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I110" s="20"/>
       <c r="J110" s="20"/>
       <c r="K110" s="20"/>
       <c r="L110" s="22"/>
       <c r="M110" s="22"/>
     </row>
-    <row r="111" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I111" s="20"/>
       <c r="J111" s="20"/>
       <c r="K111" s="20"/>
       <c r="L111" s="22"/>
       <c r="M111" s="22"/>
     </row>
-    <row r="112" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I112" s="20"/>
       <c r="J112" s="20"/>
       <c r="K112" s="20"/>
       <c r="L112" s="22"/>
       <c r="M112" s="22"/>
     </row>
-    <row r="113" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="113" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I113" s="20"/>
       <c r="J113" s="20"/>
       <c r="K113" s="20"/>
       <c r="L113" s="22"/>
       <c r="M113" s="22"/>
     </row>
-    <row r="114" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="114" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I114" s="20"/>
       <c r="J114" s="20"/>
       <c r="K114" s="20"/>
       <c r="L114" s="22"/>
       <c r="M114" s="22"/>
     </row>
-    <row r="115" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="115" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I115" s="20"/>
       <c r="J115" s="20"/>
       <c r="K115" s="20"/>
       <c r="L115" s="22"/>
       <c r="M115" s="22"/>
     </row>
-    <row r="116" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="116" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I116" s="20"/>
       <c r="J116" s="20"/>
       <c r="K116" s="20"/>
       <c r="L116" s="22"/>
       <c r="M116" s="22"/>
     </row>
-    <row r="117" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="117" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I117" s="20"/>
       <c r="J117" s="20"/>
       <c r="K117" s="20"/>
       <c r="L117" s="22"/>
       <c r="M117" s="22"/>
     </row>
-    <row r="118" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="118" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I118" s="20"/>
       <c r="J118" s="20"/>
       <c r="K118" s="20"/>
       <c r="L118" s="22"/>
       <c r="M118" s="22"/>
     </row>
-    <row r="119" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="119" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I119" s="20"/>
       <c r="J119" s="20"/>
       <c r="K119" s="20"/>
       <c r="L119" s="22"/>
       <c r="M119" s="22"/>
     </row>
-    <row r="120" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="120" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I120" s="20"/>
       <c r="J120" s="20"/>
       <c r="K120" s="20"/>
       <c r="L120" s="22"/>
       <c r="M120" s="22"/>
     </row>
-    <row r="121" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="121" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I121" s="20"/>
       <c r="J121" s="20"/>
       <c r="K121" s="20"/>
       <c r="L121" s="22"/>
       <c r="M121" s="22"/>
     </row>
-    <row r="122" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="122" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I122" s="20"/>
       <c r="J122" s="20"/>
       <c r="K122" s="20"/>
       <c r="L122" s="22"/>
       <c r="M122" s="22"/>
     </row>
-    <row r="123" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="123" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I123" s="20"/>
       <c r="J123" s="20"/>
       <c r="K123" s="20"/>
       <c r="L123" s="22"/>
       <c r="M123" s="22"/>
     </row>
-    <row r="124" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="124" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I124" s="20"/>
       <c r="J124" s="20"/>
       <c r="K124" s="20"/>
       <c r="L124" s="22"/>
       <c r="M124" s="22"/>
     </row>
-    <row r="125" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="125" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I125" s="20"/>
       <c r="J125" s="20"/>
       <c r="K125" s="20"/>
       <c r="L125" s="22"/>
       <c r="M125" s="22"/>
     </row>
-    <row r="126" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="126" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I126" s="20"/>
       <c r="J126" s="20"/>
       <c r="K126" s="20"/>
       <c r="L126" s="22"/>
       <c r="M126" s="22"/>
     </row>
-    <row r="127" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="127" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I127" s="20"/>
       <c r="J127" s="20"/>
       <c r="K127" s="20"/>
       <c r="L127" s="22"/>
       <c r="M127" s="22"/>
     </row>
-    <row r="128" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="128" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I128" s="20"/>
       <c r="J128" s="20"/>
       <c r="K128" s="20"/>
       <c r="L128" s="22"/>
       <c r="M128" s="22"/>
     </row>
-    <row r="129" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="129" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I129" s="20"/>
       <c r="J129" s="20"/>
       <c r="K129" s="20"/>
       <c r="L129" s="22"/>
       <c r="M129" s="22"/>
     </row>
-    <row r="130" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="130" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I130" s="20"/>
       <c r="J130" s="20"/>
       <c r="K130" s="20"/>
       <c r="L130" s="22"/>
       <c r="M130" s="22"/>
     </row>
-    <row r="131" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="131" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I131" s="20"/>
       <c r="J131" s="20"/>
       <c r="K131" s="20"/>
       <c r="L131" s="22"/>
       <c r="M131" s="22"/>
     </row>
-    <row r="132" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="132" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I132" s="20"/>
       <c r="J132" s="20"/>
       <c r="K132" s="20"/>
       <c r="L132" s="22"/>
       <c r="M132" s="22"/>
     </row>
-    <row r="133" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="133" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I133" s="20"/>
       <c r="J133" s="20"/>
       <c r="K133" s="20"/>
       <c r="L133" s="22"/>
       <c r="M133" s="22"/>
     </row>
-    <row r="134" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="134" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I134" s="20"/>
       <c r="J134" s="20"/>
       <c r="K134" s="20"/>
       <c r="L134" s="22"/>
       <c r="M134" s="22"/>
     </row>
-    <row r="135" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="135" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I135" s="20"/>
       <c r="J135" s="20"/>
       <c r="K135" s="20"/>
       <c r="L135" s="22"/>
       <c r="M135" s="22"/>
     </row>
-    <row r="136" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="136" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I136" s="20"/>
       <c r="J136" s="20"/>
       <c r="K136" s="20"/>
       <c r="L136" s="22"/>
       <c r="M136" s="22"/>
     </row>
-    <row r="137" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="137" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I137" s="20"/>
       <c r="J137" s="20"/>
       <c r="K137" s="20"/>
       <c r="L137" s="22"/>
       <c r="M137" s="22"/>
     </row>
-    <row r="138" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="138" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I138" s="20"/>
       <c r="J138" s="20"/>
       <c r="K138" s="20"/>
       <c r="L138" s="22"/>
       <c r="M138" s="22"/>
     </row>
-    <row r="139" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="139" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I139" s="20"/>
       <c r="J139" s="20"/>
       <c r="K139" s="20"/>
       <c r="L139" s="22"/>
       <c r="M139" s="22"/>
     </row>
-    <row r="140" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="140" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I140" s="20"/>
       <c r="J140" s="20"/>
       <c r="K140" s="20"/>
       <c r="L140" s="22"/>
       <c r="M140" s="22"/>
     </row>
-    <row r="141" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="141" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I141" s="20"/>
       <c r="J141" s="20"/>
       <c r="K141" s="20"/>
       <c r="L141" s="22"/>
       <c r="M141" s="22"/>
     </row>
-    <row r="142" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="142" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I142" s="20"/>
       <c r="J142" s="20"/>
       <c r="K142" s="20"/>
       <c r="L142" s="22"/>
       <c r="M142" s="22"/>
     </row>
-    <row r="143" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="143" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I143" s="20"/>
       <c r="J143" s="20"/>
       <c r="K143" s="20"/>
       <c r="L143" s="22"/>
       <c r="M143" s="22"/>
     </row>
-    <row r="144" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="144" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I144" s="20"/>
       <c r="J144" s="20"/>
       <c r="K144" s="20"/>
       <c r="L144" s="22"/>
       <c r="M144" s="22"/>
     </row>
-    <row r="145" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="145" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I145" s="20"/>
       <c r="J145" s="20"/>
       <c r="K145" s="20"/>
       <c r="L145" s="22"/>
       <c r="M145" s="22"/>
     </row>
-    <row r="146" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="146" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I146" s="20"/>
       <c r="J146" s="20"/>
       <c r="K146" s="20"/>
       <c r="L146" s="22"/>
       <c r="M146" s="22"/>
     </row>
-    <row r="147" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="147" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I147" s="20"/>
       <c r="J147" s="20"/>
       <c r="K147" s="20"/>
       <c r="L147" s="22"/>
       <c r="M147" s="22"/>
     </row>
-    <row r="148" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="148" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I148" s="20"/>
       <c r="J148" s="20"/>
       <c r="K148" s="20"/>
       <c r="L148" s="22"/>
       <c r="M148" s="22"/>
     </row>
-    <row r="149" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="149" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I149" s="20"/>
       <c r="J149" s="20"/>
       <c r="K149" s="20"/>
       <c r="L149" s="22"/>
       <c r="M149" s="22"/>
     </row>
-    <row r="150" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="150" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I150" s="20"/>
       <c r="J150" s="20"/>
       <c r="K150" s="20"/>
       <c r="L150" s="22"/>
       <c r="M150" s="22"/>
     </row>
-    <row r="151" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="151" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I151" s="20"/>
       <c r="J151" s="20"/>
       <c r="K151" s="20"/>
       <c r="L151" s="22"/>
       <c r="M151" s="22"/>
     </row>
-    <row r="152" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="152" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I152" s="20"/>
       <c r="J152" s="20"/>
       <c r="K152" s="20"/>
       <c r="L152" s="22"/>
       <c r="M152" s="22"/>
     </row>
-    <row r="153" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="153" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I153" s="20"/>
       <c r="J153" s="20"/>
       <c r="K153" s="20"/>
       <c r="L153" s="22"/>
       <c r="M153" s="22"/>
     </row>
-    <row r="154" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="154" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I154" s="20"/>
       <c r="J154" s="20"/>
       <c r="K154" s="20"/>
       <c r="L154" s="22"/>
       <c r="M154" s="22"/>
     </row>
-    <row r="155" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="155" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I155" s="20"/>
       <c r="J155" s="20"/>
       <c r="K155" s="20"/>
       <c r="L155" s="22"/>
       <c r="M155" s="22"/>
     </row>
-    <row r="156" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="156" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I156" s="20"/>
       <c r="J156" s="20"/>
       <c r="K156" s="20"/>
       <c r="L156" s="22"/>
       <c r="M156" s="22"/>
     </row>
-    <row r="157" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="157" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I157" s="20"/>
       <c r="J157" s="20"/>
       <c r="K157" s="20"/>
       <c r="L157" s="22"/>
       <c r="M157" s="22"/>
     </row>
-    <row r="158" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="158" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I158" s="20"/>
       <c r="J158" s="20"/>
       <c r="K158" s="20"/>
       <c r="L158" s="22"/>
       <c r="M158" s="22"/>
     </row>
-    <row r="159" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="159" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I159" s="20"/>
       <c r="J159" s="20"/>
       <c r="K159" s="20"/>
       <c r="L159" s="22"/>
       <c r="M159" s="22"/>
     </row>
-    <row r="160" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="160" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I160" s="20"/>
       <c r="J160" s="20"/>
       <c r="K160" s="20"/>
       <c r="L160" s="22"/>
       <c r="M160" s="22"/>
     </row>
-    <row r="161" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="161" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I161" s="20"/>
       <c r="J161" s="20"/>
       <c r="K161" s="20"/>
       <c r="L161" s="22"/>
       <c r="M161" s="22"/>
     </row>
-    <row r="162" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="162" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I162" s="20"/>
       <c r="J162" s="20"/>
       <c r="K162" s="20"/>
       <c r="L162" s="22"/>
       <c r="M162" s="22"/>
     </row>
-    <row r="163" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="163" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I163" s="20"/>
       <c r="J163" s="20"/>
       <c r="K163" s="20"/>
       <c r="L163" s="22"/>
       <c r="M163" s="22"/>
     </row>
-    <row r="164" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="164" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I164" s="20"/>
       <c r="J164" s="20"/>
       <c r="K164" s="20"/>
       <c r="L164" s="22"/>
       <c r="M164" s="22"/>
     </row>
-    <row r="165" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="165" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I165" s="20"/>
       <c r="J165" s="20"/>
       <c r="K165" s="20"/>
       <c r="L165" s="22"/>
       <c r="M165" s="22"/>
     </row>
-    <row r="166" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="166" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I166" s="20"/>
       <c r="J166" s="20"/>
       <c r="K166" s="20"/>
       <c r="L166" s="22"/>
       <c r="M166" s="22"/>
     </row>
-    <row r="167" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="167" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I167" s="20"/>
       <c r="J167" s="20"/>
       <c r="K167" s="20"/>
       <c r="L167" s="22"/>
       <c r="M167" s="22"/>
     </row>
-    <row r="168" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="168" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I168" s="20"/>
       <c r="J168" s="20"/>
       <c r="K168" s="20"/>
       <c r="L168" s="22"/>
       <c r="M168" s="22"/>
     </row>
-    <row r="169" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="169" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I169" s="20"/>
       <c r="J169" s="20"/>
       <c r="K169" s="20"/>
       <c r="L169" s="22"/>
       <c r="M169" s="22"/>
     </row>
-    <row r="170" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="170" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I170" s="20"/>
       <c r="J170" s="20"/>
       <c r="K170" s="20"/>
       <c r="L170" s="22"/>
       <c r="M170" s="22"/>
     </row>
-    <row r="171" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="171" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I171" s="20"/>
       <c r="J171" s="20"/>
       <c r="K171" s="20"/>
       <c r="L171" s="22"/>
       <c r="M171" s="22"/>
     </row>
-    <row r="172" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="172" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I172" s="20"/>
       <c r="J172" s="20"/>
       <c r="K172" s="20"/>
       <c r="L172" s="22"/>
       <c r="M172" s="22"/>
     </row>
-    <row r="173" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="173" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I173" s="20"/>
       <c r="J173" s="20"/>
       <c r="K173" s="20"/>
       <c r="L173" s="22"/>
       <c r="M173" s="22"/>
     </row>
-    <row r="174" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="174" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I174" s="20"/>
       <c r="J174" s="20"/>
       <c r="K174" s="20"/>
       <c r="L174" s="22"/>
       <c r="M174" s="22"/>
     </row>
-    <row r="175" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="175" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I175" s="20"/>
       <c r="J175" s="20"/>
       <c r="K175" s="20"/>
       <c r="L175" s="22"/>
       <c r="M175" s="22"/>
     </row>
-    <row r="176" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="176" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I176" s="20"/>
       <c r="J176" s="20"/>
       <c r="K176" s="20"/>
       <c r="L176" s="22"/>
       <c r="M176" s="22"/>
     </row>
-    <row r="177" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="177" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I177" s="20"/>
       <c r="J177" s="20"/>
       <c r="K177" s="20"/>
       <c r="L177" s="22"/>
       <c r="M177" s="22"/>
     </row>
-    <row r="178" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="178" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I178" s="20"/>
       <c r="J178" s="20"/>
       <c r="K178" s="20"/>
       <c r="L178" s="22"/>
       <c r="M178" s="22"/>
     </row>
-    <row r="179" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="179" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I179" s="20"/>
       <c r="J179" s="20"/>
       <c r="K179" s="20"/>
       <c r="L179" s="22"/>
       <c r="M179" s="22"/>
     </row>
-    <row r="180" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="180" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I180" s="20"/>
       <c r="J180" s="20"/>
       <c r="K180" s="20"/>
       <c r="L180" s="22"/>
       <c r="M180" s="22"/>
     </row>
-    <row r="181" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="181" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I181" s="20"/>
       <c r="J181" s="20"/>
       <c r="K181" s="20"/>
       <c r="L181" s="22"/>
       <c r="M181" s="22"/>
     </row>
-    <row r="182" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="182" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I182" s="20"/>
       <c r="J182" s="20"/>
       <c r="K182" s="20"/>
       <c r="L182" s="22"/>
       <c r="M182" s="22"/>
     </row>
-    <row r="183" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="183" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I183" s="20"/>
       <c r="J183" s="20"/>
       <c r="K183" s="20"/>
       <c r="L183" s="22"/>
       <c r="M183" s="22"/>
     </row>
-    <row r="184" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="184" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I184" s="20"/>
       <c r="J184" s="20"/>
       <c r="K184" s="20"/>
       <c r="L184" s="22"/>
       <c r="M184" s="22"/>
     </row>
-    <row r="185" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="185" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I185" s="20"/>
       <c r="J185" s="20"/>
       <c r="K185" s="20"/>
       <c r="L185" s="22"/>
       <c r="M185" s="22"/>
     </row>
-    <row r="186" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="186" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I186" s="20"/>
       <c r="J186" s="20"/>
       <c r="K186" s="20"/>
       <c r="L186" s="22"/>
       <c r="M186" s="22"/>
     </row>
-    <row r="187" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="187" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I187" s="20"/>
       <c r="J187" s="20"/>
       <c r="K187" s="20"/>
       <c r="L187" s="22"/>
       <c r="M187" s="22"/>
     </row>
-    <row r="188" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="188" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I188" s="20"/>
       <c r="J188" s="20"/>
       <c r="K188" s="20"/>
       <c r="L188" s="22"/>
       <c r="M188" s="22"/>
     </row>
-    <row r="189" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I189" s="20"/>
       <c r="J189" s="20"/>
       <c r="K189" s="20"/>
       <c r="L189" s="22"/>
       <c r="M189" s="22"/>
     </row>
-    <row r="190" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="190" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I190" s="20"/>
       <c r="J190" s="20"/>
       <c r="K190" s="20"/>
       <c r="L190" s="22"/>
       <c r="M190" s="22"/>
     </row>
-    <row r="191" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="191" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I191" s="20"/>
       <c r="J191" s="20"/>
       <c r="K191" s="20"/>
       <c r="L191" s="22"/>
       <c r="M191" s="22"/>
     </row>
-    <row r="192" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="192" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I192" s="20"/>
       <c r="J192" s="20"/>
       <c r="K192" s="20"/>
       <c r="L192" s="22"/>
       <c r="M192" s="22"/>
     </row>
-    <row r="193" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="193" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I193" s="20"/>
       <c r="J193" s="20"/>
       <c r="K193" s="20"/>
       <c r="L193" s="22"/>
       <c r="M193" s="22"/>
     </row>
-    <row r="194" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="194" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I194" s="20"/>
       <c r="J194" s="20"/>
       <c r="K194" s="20"/>
       <c r="L194" s="22"/>
       <c r="M194" s="22"/>
     </row>
-    <row r="195" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="195" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I195" s="20"/>
       <c r="J195" s="20"/>
       <c r="K195" s="20"/>
       <c r="L195" s="22"/>
       <c r="M195" s="22"/>
     </row>
-    <row r="196" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="196" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I196" s="20"/>
       <c r="J196" s="20"/>
       <c r="K196" s="20"/>
       <c r="L196" s="22"/>
       <c r="M196" s="22"/>
     </row>
-    <row r="197" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="197" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I197" s="20"/>
       <c r="J197" s="20"/>
       <c r="K197" s="20"/>
       <c r="L197" s="22"/>
       <c r="M197" s="22"/>
     </row>
-    <row r="198" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="198" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I198" s="20"/>
       <c r="J198" s="20"/>
       <c r="K198" s="20"/>
       <c r="L198" s="22"/>
       <c r="M198" s="22"/>
     </row>
-    <row r="199" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="199" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I199" s="20"/>
       <c r="J199" s="20"/>
       <c r="K199" s="20"/>
       <c r="L199" s="22"/>
       <c r="M199" s="22"/>
     </row>
-    <row r="200" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="200" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I200" s="20"/>
       <c r="J200" s="20"/>
       <c r="K200" s="20"/>
       <c r="L200" s="22"/>
       <c r="M200" s="22"/>
     </row>
-    <row r="201" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="201" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I201" s="20"/>
       <c r="J201" s="20"/>
       <c r="K201" s="20"/>
       <c r="L201" s="22"/>
       <c r="M201" s="22"/>
     </row>
-    <row r="202" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="202" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I202" s="20"/>
       <c r="J202" s="20"/>
       <c r="K202" s="20"/>
       <c r="L202" s="22"/>
       <c r="M202" s="22"/>
     </row>
-    <row r="203" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="203" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I203" s="20"/>
       <c r="J203" s="20"/>
       <c r="K203" s="20"/>
       <c r="L203" s="22"/>
       <c r="M203" s="22"/>
     </row>
-    <row r="204" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="204" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I204" s="20"/>
       <c r="J204" s="20"/>
       <c r="K204" s="20"/>
       <c r="L204" s="22"/>
       <c r="M204" s="22"/>
     </row>
-    <row r="205" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="205" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I205" s="20"/>
       <c r="J205" s="20"/>
       <c r="K205" s="20"/>
       <c r="L205" s="22"/>
       <c r="M205" s="22"/>
     </row>
-    <row r="206" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="206" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I206" s="20"/>
       <c r="J206" s="20"/>
       <c r="K206" s="20"/>
       <c r="L206" s="22"/>
       <c r="M206" s="22"/>
     </row>
-    <row r="207" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="207" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I207" s="20"/>
       <c r="J207" s="20"/>
       <c r="K207" s="20"/>
       <c r="L207" s="22"/>
       <c r="M207" s="22"/>
     </row>
-    <row r="208" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="208" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I208" s="20"/>
       <c r="J208" s="20"/>
       <c r="K208" s="20"/>
       <c r="L208" s="22"/>
       <c r="M208" s="22"/>
     </row>
-    <row r="209" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I209" s="20"/>
       <c r="J209" s="20"/>
       <c r="K209" s="20"/>
       <c r="L209" s="22"/>
       <c r="M209" s="22"/>
     </row>
-    <row r="210" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I210" s="20"/>
       <c r="J210" s="20"/>
       <c r="K210" s="20"/>
       <c r="L210" s="22"/>
       <c r="M210" s="22"/>
     </row>
-    <row r="211" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I211" s="20"/>
       <c r="J211" s="20"/>
       <c r="K211" s="20"/>
       <c r="L211" s="22"/>
       <c r="M211" s="22"/>
     </row>
-    <row r="212" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I212" s="20"/>
       <c r="J212" s="20"/>
       <c r="K212" s="20"/>
       <c r="L212" s="22"/>
       <c r="M212" s="22"/>
     </row>
-    <row r="213" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I213" s="20"/>
       <c r="J213" s="20"/>
       <c r="K213" s="20"/>
       <c r="L213" s="22"/>
       <c r="M213" s="22"/>
     </row>
-    <row r="214" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I214" s="20"/>
       <c r="J214" s="20"/>
       <c r="K214" s="20"/>
       <c r="L214" s="22"/>
       <c r="M214" s="22"/>
     </row>
-    <row r="215" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I215" s="20"/>
       <c r="J215" s="20"/>
       <c r="K215" s="20"/>
       <c r="L215" s="22"/>
       <c r="M215" s="22"/>
     </row>
-    <row r="216" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I216" s="20"/>
       <c r="J216" s="20"/>
       <c r="K216" s="20"/>
       <c r="L216" s="22"/>
       <c r="M216" s="22"/>
     </row>
-    <row r="217" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I217" s="20"/>
       <c r="J217" s="20"/>
       <c r="K217" s="20"/>
       <c r="L217" s="22"/>
       <c r="M217" s="22"/>
     </row>
-    <row r="218" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I218" s="20"/>
       <c r="J218" s="20"/>
       <c r="K218" s="20"/>
       <c r="L218" s="22"/>
       <c r="M218" s="22"/>
     </row>
-    <row r="219" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I219" s="20"/>
       <c r="J219" s="20"/>
       <c r="K219" s="20"/>
       <c r="L219" s="22"/>
       <c r="M219" s="22"/>
     </row>
-    <row r="220" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I220" s="20"/>
       <c r="J220" s="20"/>
       <c r="K220" s="20"/>
       <c r="L220" s="22"/>
       <c r="M220" s="22"/>
     </row>
-    <row r="221" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I221" s="20"/>
       <c r="J221" s="20"/>
       <c r="K221" s="20"/>
       <c r="L221" s="22"/>
       <c r="M221" s="22"/>
     </row>
-    <row r="222" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I222" s="20"/>
       <c r="J222" s="20"/>
       <c r="K222" s="20"/>
       <c r="L222" s="22"/>
       <c r="M222" s="22"/>
     </row>
-    <row r="223" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I223" s="20"/>
       <c r="J223" s="20"/>
       <c r="K223" s="20"/>
       <c r="L223" s="22"/>
       <c r="M223" s="22"/>
     </row>
-    <row r="224" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I224" s="20"/>
       <c r="J224" s="20"/>
       <c r="K224" s="20"/>
       <c r="L224" s="22"/>
       <c r="M224" s="22"/>
     </row>
-    <row r="225" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I225" s="20"/>
       <c r="J225" s="20"/>
       <c r="K225" s="20"/>
       <c r="L225" s="22"/>
       <c r="M225" s="22"/>
     </row>
-    <row r="226" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I226" s="20"/>
       <c r="J226" s="20"/>
       <c r="K226" s="20"/>
       <c r="L226" s="22"/>
       <c r="M226" s="22"/>
     </row>
-    <row r="227" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I227" s="20"/>
       <c r="J227" s="20"/>
       <c r="K227" s="20"/>
       <c r="L227" s="22"/>
       <c r="M227" s="22"/>
     </row>
-    <row r="228" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I228" s="20"/>
       <c r="J228" s="20"/>
       <c r="K228" s="20"/>
       <c r="L228" s="22"/>
       <c r="M228" s="22"/>
     </row>
-    <row r="229" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I229" s="20"/>
       <c r="J229" s="20"/>
       <c r="K229" s="20"/>
       <c r="L229" s="22"/>
       <c r="M229" s="22"/>
     </row>
-    <row r="230" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I230" s="20"/>
       <c r="J230" s="20"/>
       <c r="K230" s="20"/>
       <c r="L230" s="22"/>
       <c r="M230" s="22"/>
     </row>
-    <row r="231" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I231" s="20"/>
       <c r="J231" s="20"/>
       <c r="K231" s="20"/>
       <c r="L231" s="22"/>
       <c r="M231" s="22"/>
     </row>
-    <row r="232" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I232" s="20"/>
       <c r="J232" s="20"/>
       <c r="K232" s="20"/>
       <c r="L232" s="22"/>
       <c r="M232" s="22"/>
     </row>
-    <row r="233" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I233" s="20"/>
       <c r="J233" s="20"/>
       <c r="K233" s="20"/>
       <c r="L233" s="22"/>
       <c r="M233" s="22"/>
     </row>
-    <row r="234" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I234" s="20"/>
       <c r="J234" s="20"/>
       <c r="K234" s="20"/>
     </row>
-    <row r="235" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I235" s="20"/>
       <c r="J235" s="20"/>
       <c r="K235" s="20"/>
     </row>
-    <row r="236" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I236" s="20"/>
       <c r="J236" s="20"/>
       <c r="K236" s="20"/>
     </row>
-    <row r="237" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I237" s="20"/>
       <c r="J237" s="20"/>
       <c r="K237" s="20"/>
     </row>
-    <row r="238" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I238" s="20"/>
       <c r="J238" s="20"/>
       <c r="K238" s="20"/>
     </row>
-    <row r="239" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I239" s="20"/>
       <c r="J239" s="20"/>
       <c r="K239" s="20"/>
     </row>
-    <row r="240" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="9:13" x14ac:dyDescent="0.45">
       <c r="I240" s="20"/>
       <c r="J240" s="20"/>
       <c r="K240" s="20"/>
     </row>
-    <row r="241" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="241" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I241" s="20"/>
       <c r="J241" s="20"/>
       <c r="K241" s="20"/>
     </row>
-    <row r="242" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="242" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I242" s="20"/>
       <c r="J242" s="20"/>
       <c r="K242" s="20"/>
     </row>
-    <row r="243" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="243" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I243" s="20"/>
       <c r="J243" s="20"/>
       <c r="K243" s="20"/>
     </row>
-    <row r="244" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="244" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I244" s="20"/>
       <c r="J244" s="20"/>
       <c r="K244" s="20"/>
     </row>
-    <row r="245" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="245" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I245" s="20"/>
       <c r="J245" s="20"/>
       <c r="K245" s="20"/>
     </row>
-    <row r="246" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="246" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I246" s="20"/>
       <c r="J246" s="20"/>
       <c r="K246" s="20"/>
     </row>
-    <row r="247" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="247" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I247" s="20"/>
       <c r="J247" s="20"/>
       <c r="K247" s="20"/>
     </row>
-    <row r="248" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="248" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I248" s="20"/>
       <c r="J248" s="20"/>
       <c r="K248" s="20"/>
     </row>
-    <row r="249" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="249" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I249" s="20"/>
       <c r="J249" s="20"/>
       <c r="K249" s="20"/>
     </row>
-    <row r="250" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="250" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I250" s="20"/>
       <c r="J250" s="20"/>
       <c r="K250" s="20"/>
     </row>
-    <row r="251" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="251" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I251" s="20"/>
       <c r="J251" s="20"/>
       <c r="K251" s="20"/>
     </row>
-    <row r="252" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="252" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I252" s="20"/>
       <c r="J252" s="20"/>
       <c r="K252" s="20"/>
     </row>
-    <row r="253" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="253" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I253" s="20"/>
       <c r="J253" s="20"/>
       <c r="K253" s="20"/>
     </row>
-    <row r="254" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="254" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I254" s="20"/>
       <c r="J254" s="20"/>
       <c r="K254" s="20"/>
     </row>
-    <row r="255" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="255" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I255" s="20"/>
       <c r="J255" s="20"/>
       <c r="K255" s="20"/>
     </row>
-    <row r="256" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="256" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I256" s="20"/>
       <c r="J256" s="20"/>
       <c r="K256" s="20"/>
     </row>
-    <row r="257" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="257" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I257" s="20"/>
       <c r="J257" s="20"/>
       <c r="K257" s="20"/>
     </row>
-    <row r="258" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="258" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I258" s="20"/>
       <c r="J258" s="20"/>
       <c r="K258" s="20"/>
     </row>
-    <row r="259" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="259" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I259" s="20"/>
       <c r="J259" s="20"/>
       <c r="K259" s="20"/>
     </row>
-    <row r="260" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="260" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I260" s="20"/>
       <c r="J260" s="20"/>
       <c r="K260" s="20"/>
     </row>
-    <row r="261" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="261" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I261" s="20"/>
       <c r="J261" s="20"/>
       <c r="K261" s="20"/>
     </row>
-    <row r="262" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="262" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I262" s="20"/>
       <c r="J262" s="20"/>
       <c r="K262" s="20"/>
     </row>
-    <row r="263" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="263" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I263" s="20"/>
       <c r="J263" s="20"/>
       <c r="K263" s="20"/>
     </row>
-    <row r="264" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="264" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I264" s="20"/>
       <c r="J264" s="20"/>
       <c r="K264" s="20"/>
     </row>
-    <row r="265" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="265" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I265" s="20"/>
       <c r="J265" s="20"/>
       <c r="K265" s="20"/>
     </row>
-    <row r="266" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="266" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I266" s="20"/>
       <c r="J266" s="20"/>
       <c r="K266" s="20"/>
     </row>
-    <row r="267" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="267" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I267" s="20"/>
       <c r="J267" s="20"/>
       <c r="K267" s="20"/>
     </row>
-    <row r="268" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="268" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I268" s="20"/>
       <c r="J268" s="20"/>
       <c r="K268" s="20"/>
     </row>
-    <row r="269" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="269" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I269" s="20"/>
       <c r="J269" s="20"/>
       <c r="K269" s="20"/>
     </row>
-    <row r="270" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="270" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I270" s="20"/>
       <c r="J270" s="20"/>
       <c r="K270" s="20"/>
     </row>
-    <row r="271" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="271" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I271" s="20"/>
       <c r="J271" s="20"/>
       <c r="K271" s="20"/>
     </row>
-    <row r="272" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="272" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I272" s="20"/>
       <c r="J272" s="20"/>
       <c r="K272" s="20"/>
     </row>
-    <row r="273" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="273" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I273" s="20"/>
       <c r="J273" s="20"/>
       <c r="K273" s="20"/>
     </row>
-    <row r="274" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="274" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I274" s="20"/>
       <c r="J274" s="20"/>
       <c r="K274" s="20"/>
     </row>
-    <row r="275" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="275" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I275" s="20"/>
       <c r="J275" s="20"/>
       <c r="K275" s="20"/>
     </row>
-    <row r="276" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="276" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I276" s="20"/>
       <c r="J276" s="20"/>
       <c r="K276" s="20"/>
     </row>
-    <row r="277" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="277" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I277" s="20"/>
       <c r="J277" s="20"/>
       <c r="K277" s="20"/>
     </row>
-    <row r="278" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="278" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I278" s="20"/>
       <c r="J278" s="20"/>
       <c r="K278" s="20"/>
     </row>
-    <row r="279" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="279" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I279" s="20"/>
       <c r="J279" s="20"/>
       <c r="K279" s="20"/>
     </row>
-    <row r="280" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="280" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I280" s="20"/>
       <c r="J280" s="20"/>
       <c r="K280" s="20"/>
     </row>
-    <row r="281" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="281" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I281" s="20"/>
       <c r="J281" s="20"/>
       <c r="K281" s="20"/>
     </row>
-    <row r="282" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="282" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I282" s="20"/>
       <c r="J282" s="20"/>
       <c r="K282" s="20"/>
     </row>
-    <row r="283" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="283" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I283" s="20"/>
       <c r="J283" s="20"/>
       <c r="K283" s="20"/>
     </row>
-    <row r="284" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="284" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I284" s="20"/>
       <c r="J284" s="20"/>
       <c r="K284" s="20"/>
     </row>
-    <row r="285" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="285" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I285" s="20"/>
       <c r="J285" s="20"/>
       <c r="K285" s="20"/>
     </row>
-    <row r="286" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="286" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I286" s="20"/>
       <c r="J286" s="20"/>
       <c r="K286" s="20"/>
     </row>
-    <row r="287" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="287" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I287" s="20"/>
       <c r="J287" s="20"/>
       <c r="K287" s="20"/>
     </row>
-    <row r="288" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="288" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I288" s="20"/>
       <c r="J288" s="20"/>
       <c r="K288" s="20"/>
     </row>
-    <row r="289" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="289" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I289" s="20"/>
       <c r="J289" s="20"/>
       <c r="K289" s="20"/>
     </row>
-    <row r="290" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="290" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I290" s="20"/>
       <c r="J290" s="20"/>
       <c r="K290" s="20"/>
     </row>
-    <row r="291" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="291" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I291" s="20"/>
       <c r="J291" s="20"/>
       <c r="K291" s="20"/>
     </row>
-    <row r="292" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="292" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I292" s="20"/>
       <c r="J292" s="20"/>
       <c r="K292" s="20"/>
     </row>
-    <row r="293" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="293" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I293" s="20"/>
       <c r="J293" s="20"/>
       <c r="K293" s="20"/>
     </row>
-    <row r="294" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="294" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I294" s="20"/>
       <c r="J294" s="20"/>
       <c r="K294" s="20"/>
     </row>
-    <row r="295" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="295" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I295" s="20"/>
       <c r="J295" s="20"/>
       <c r="K295" s="20"/>
     </row>
-    <row r="296" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="296" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I296" s="20"/>
       <c r="J296" s="20"/>
       <c r="K296" s="20"/>
     </row>
-    <row r="297" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="297" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I297" s="20"/>
       <c r="J297" s="20"/>
       <c r="K297" s="20"/>
     </row>
-    <row r="298" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="298" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I298" s="20"/>
       <c r="J298" s="20"/>
       <c r="K298" s="20"/>
     </row>
-    <row r="299" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="299" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I299" s="20"/>
       <c r="J299" s="20"/>
       <c r="K299" s="20"/>
     </row>
-    <row r="300" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="300" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I300" s="20"/>
       <c r="J300" s="20"/>
       <c r="K300" s="20"/>
     </row>
-    <row r="301" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="301" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I301" s="20"/>
       <c r="J301" s="20"/>
       <c r="K301" s="20"/>
     </row>
-    <row r="302" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="302" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I302" s="20"/>
       <c r="J302" s="20"/>
       <c r="K302" s="20"/>
     </row>
-    <row r="303" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="303" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I303" s="20"/>
       <c r="J303" s="20"/>
       <c r="K303" s="20"/>
     </row>
-    <row r="304" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="304" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I304" s="20"/>
       <c r="J304" s="20"/>
       <c r="K304" s="20"/>
     </row>
-    <row r="305" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="305" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I305" s="20"/>
       <c r="J305" s="20"/>
       <c r="K305" s="20"/>
     </row>
-    <row r="306" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="306" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I306" s="20"/>
       <c r="J306" s="20"/>
       <c r="K306" s="20"/>
     </row>
-    <row r="307" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="307" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I307" s="20"/>
       <c r="J307" s="20"/>
       <c r="K307" s="20"/>
     </row>
-    <row r="308" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="308" spans="9:11" x14ac:dyDescent="0.45">
       <c r="I308" s="20"/>
       <c r="J308" s="20"/>
       <c r="K308" s="20"/>
@@ -30515,25 +30521,25 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U24"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L19" sqref="L19"/>
-      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
+      <selection pane="bottomLeft" activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30556,7 +30562,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>43</v>
@@ -30581,7 +30587,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -30606,7 +30612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30629,14 +30635,24 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
-    <row r="23" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="18:18" x14ac:dyDescent="0.45">
       <c r="R23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="18:18" x14ac:dyDescent="0.45">
       <c r="R24" s="1" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="18:18" x14ac:dyDescent="0.45">
+      <c r="R26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="18:18" x14ac:dyDescent="0.45">
+      <c r="R27" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -30659,17 +30675,17 @@
       <selection pane="bottomLeft" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30692,7 +30708,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>38</v>
@@ -30717,7 +30733,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>28</v>
@@ -30744,7 +30760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30787,17 +30803,17 @@
       <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="1"/>
-    <col min="3" max="7" width="11.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" style="2" customWidth="1"/>
-    <col min="9" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="2.73046875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" style="1"/>
+    <col min="3" max="7" width="11.3984375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.3984375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30820,7 +30836,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>39</v>
@@ -30845,7 +30861,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="s">
         <v>42</v>
@@ -30872,7 +30888,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>
@@ -30895,7 +30911,7 @@
       <c r="T4" s="24"/>
       <c r="U4" s="24"/>
     </row>
-    <row r="45" ht="57.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="57.75" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -30915,12 +30931,12 @@
       <selection pane="bottomLeft" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="45"/>
       <c r="B1" s="48"/>
       <c r="C1" s="3"/>
@@ -30943,7 +30959,7 @@
       <c r="T1" s="24"/>
       <c r="U1" s="24"/>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="45"/>
       <c r="B2" s="6" t="s">
         <v>27</v>
@@ -30968,7 +30984,7 @@
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
     </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A3" s="45"/>
       <c r="B3" s="7" t="str">
         <f>Übersicht!B3</f>
@@ -30996,7 +31012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="45"/>
       <c r="B4" s="48"/>
       <c r="C4" s="3"/>

</xml_diff>